<commit_message>
Konsole wird nicht geöffnet, Excel ist hidden
</commit_message>
<xml_diff>
--- a/Schrauben/Tabelle-Werte.xlsx
+++ b/Schrauben/Tabelle-Werte.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edisd\Desktop\Edis\Studiengang\Semestar III\Hochsprachenprogramierung\Labor\Workspace\HSP-SoSe-2021\Schrauben\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Machina\Desktop\Studium\3. Semester\HSP\Repositories\HSP-SoSe-2021\Schrauben\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C76223E-3647-4829-9949-5803F6695C24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320CC625-0078-42BC-B78D-CB7E7EB8ADC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EC6E8927-7B9C-45F5-9187-D380C00F6962}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EC6E8927-7B9C-45F5-9187-D380C00F6962}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -907,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE13EF1-61C1-43B8-92FA-015A68CF7169}">
   <dimension ref="A1:BC66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5890,6 +5890,6 @@
     <mergeCell ref="C65:G65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel gibt Kopfmaße aus
</commit_message>
<xml_diff>
--- a/Schrauben/Tabelle-Werte.xlsx
+++ b/Schrauben/Tabelle-Werte.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Desktop\Hochsprachenprogrammierung\Sprint\HSP-SoSe-2021\Schrauben\Schrauben\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Desktop\Hochsprachenprogrammierung\Sprint\HSP-SoSe-2021\Schrauben\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28BBA92-AA1C-4D45-84A4-F054A48DD6A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE11FC6-3F58-445F-B1AF-D20F48E85153}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="0" windowWidth="28740" windowHeight="15600" xr2:uid="{EC6E8927-7B9C-45F5-9187-D380C00F6962}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="116">
   <si>
     <t>Test1</t>
   </si>
@@ -376,6 +376,12 @@
   </si>
   <si>
     <t>4.6</t>
+  </si>
+  <si>
+    <t>Senk Durchmesser</t>
+  </si>
+  <si>
+    <t>Allgemein Kopfhöhe</t>
   </si>
 </sst>
 </file>
@@ -445,7 +451,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -533,29 +539,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -574,9 +562,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -586,7 +571,6 @@
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -615,6 +599,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -931,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE13EF1-61C1-43B8-92FA-015A68CF7169}">
   <dimension ref="A1:BC66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,14 +933,14 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1091,11 +1077,11 @@
       <c r="B10">
         <v>50</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1118,7 +1104,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1146,73 +1132,73 @@
       </c>
     </row>
     <row r="19" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="36"/>
-      <c r="R19" s="37" t="s">
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="S19" s="32"/>
-      <c r="T19" s="32"/>
-      <c r="U19" s="32"/>
-      <c r="V19" s="32"/>
-      <c r="W19" s="32"/>
-      <c r="X19" s="32"/>
-      <c r="Y19" s="32"/>
-      <c r="Z19" s="32"/>
-      <c r="AA19" s="32"/>
-      <c r="AB19" s="32"/>
-      <c r="AC19" s="32"/>
-      <c r="AD19" s="32"/>
-      <c r="AE19" s="32"/>
-      <c r="AF19" s="32"/>
-      <c r="AG19" s="32"/>
-      <c r="AH19" s="32"/>
-      <c r="AI19" s="32"/>
-      <c r="AJ19" s="32"/>
-      <c r="AK19" s="32"/>
-      <c r="AL19" s="32"/>
-      <c r="AM19" s="32"/>
-      <c r="AN19" s="32"/>
-      <c r="AO19" s="32"/>
-      <c r="AP19" s="32"/>
-      <c r="AQ19" s="32"/>
-      <c r="AR19" s="32"/>
-      <c r="AS19" s="32"/>
-      <c r="AT19" s="32"/>
-      <c r="AU19" s="32"/>
-      <c r="AV19" s="38"/>
-      <c r="AW19" s="31" t="s">
+      <c r="S19" s="28"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="28"/>
+      <c r="X19" s="28"/>
+      <c r="Y19" s="28"/>
+      <c r="Z19" s="28"/>
+      <c r="AA19" s="28"/>
+      <c r="AB19" s="28"/>
+      <c r="AC19" s="28"/>
+      <c r="AD19" s="28"/>
+      <c r="AE19" s="28"/>
+      <c r="AF19" s="28"/>
+      <c r="AG19" s="28"/>
+      <c r="AH19" s="28"/>
+      <c r="AI19" s="28"/>
+      <c r="AJ19" s="28"/>
+      <c r="AK19" s="28"/>
+      <c r="AL19" s="28"/>
+      <c r="AM19" s="28"/>
+      <c r="AN19" s="28"/>
+      <c r="AO19" s="28"/>
+      <c r="AP19" s="28"/>
+      <c r="AQ19" s="28"/>
+      <c r="AR19" s="28"/>
+      <c r="AS19" s="28"/>
+      <c r="AT19" s="28"/>
+      <c r="AU19" s="28"/>
+      <c r="AV19" s="34"/>
+      <c r="AW19" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="AX19" s="32"/>
-      <c r="AY19" s="32"/>
-      <c r="AZ19" s="32"/>
-      <c r="BA19" s="32"/>
-      <c r="BB19" s="32"/>
-      <c r="BC19" s="32"/>
+      <c r="AX19" s="28"/>
+      <c r="AY19" s="28"/>
+      <c r="AZ19" s="28"/>
+      <c r="BA19" s="28"/>
+      <c r="BB19" s="28"/>
+      <c r="BC19" s="28"/>
     </row>
     <row r="20" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1379,7 +1365,7 @@
       <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="19" t="str">
+      <c r="B21" s="16" t="str">
         <f>IF($B13 = "M1.6","1.6","0")</f>
         <v>0</v>
       </c>
@@ -1409,7 +1395,7 @@
       </c>
       <c r="I21" s="1" t="str">
         <f>IF($B13 = "M8","8","0")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J21" s="1" t="str">
         <f>IF($B13 = "M10","10","0")</f>
@@ -1441,7 +1427,7 @@
       </c>
       <c r="Q21" s="13" t="str">
         <f>IF($B13 = "M42","42","0")</f>
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="R21" s="15" t="str">
         <f>IF($B13 = "M2x0,25","2","0")</f>
@@ -1600,7 +1586,7 @@
       <c r="A22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="19" t="str">
+      <c r="B22" s="16" t="str">
         <f>IF(B21="0","0","0.35")</f>
         <v>0</v>
       </c>
@@ -1630,7 +1616,7 @@
       </c>
       <c r="I22" s="1" t="str">
         <f>IF(I21="0","0","1.25")</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="J22" s="1" t="str">
         <f>IF(J21="0","0","1.5")</f>
@@ -1662,7 +1648,7 @@
       </c>
       <c r="Q22" s="13" t="str">
         <f>IF(Q21="0","0","4.5")</f>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="R22" s="15" t="str">
         <f>IF(R21="0","0","0.25")</f>
@@ -1821,7 +1807,7 @@
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="16">
         <f>B21-(0.6495*B22)</f>
         <v>0</v>
       </c>
@@ -1851,7 +1837,7 @@
       </c>
       <c r="I23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.1881250000000003</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="0"/>
@@ -1883,7 +1869,7 @@
       </c>
       <c r="Q23" s="13">
         <f t="shared" si="0"/>
-        <v>39.077249999999999</v>
+        <v>0</v>
       </c>
       <c r="R23" s="15">
         <f>R21-(0.6495*R22)</f>
@@ -2042,7 +2028,7 @@
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="16">
         <f>B21 -(1.2269 * B22)</f>
         <v>0</v>
       </c>
@@ -2072,7 +2058,7 @@
       </c>
       <c r="I24" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.4663749999999993</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" si="2"/>
@@ -2104,7 +2090,7 @@
       </c>
       <c r="Q24" s="13">
         <f t="shared" si="2"/>
-        <v>36.478949999999998</v>
+        <v>0</v>
       </c>
       <c r="R24" s="15">
         <f>R21 -(1.2269 * R22)</f>
@@ -2263,7 +2249,7 @@
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="16">
         <f>B21-B22</f>
         <v>0</v>
       </c>
@@ -2293,7 +2279,7 @@
       </c>
       <c r="I25" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" si="4"/>
@@ -2325,7 +2311,7 @@
       </c>
       <c r="Q25" s="13">
         <f t="shared" si="4"/>
-        <v>37.5</v>
+        <v>0</v>
       </c>
       <c r="R25" s="15">
         <f>R21-R22</f>
@@ -2484,7 +2470,7 @@
       <c r="A26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="17">
         <f>(PI()*(B21*B21*B21*B21))/64</f>
         <v>0</v>
       </c>
@@ -2514,7 +2500,7 @@
       </c>
       <c r="I26">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>201.06192982974676</v>
       </c>
       <c r="J26">
         <f t="shared" si="6"/>
@@ -2546,129 +2532,129 @@
       </c>
       <c r="Q26">
         <f t="shared" si="6"/>
-        <v>152745.02021569913</v>
-      </c>
-      <c r="R26" s="16">
+        <v>0</v>
+      </c>
+      <c r="R26" s="15">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="S26" s="17">
+      <c r="S26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T26" s="17">
+      <c r="T26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="U26" s="17">
+      <c r="U26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="V26" s="17">
+      <c r="V26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W26" s="17">
+      <c r="W26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X26" s="17">
+      <c r="X26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Y26" s="17">
+      <c r="Y26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Z26" s="17">
+      <c r="Z26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA26" s="17">
+      <c r="AA26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AB26" s="17">
+      <c r="AB26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AC26" s="17">
+      <c r="AC26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AD26" s="17">
+      <c r="AD26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AE26" s="17">
+      <c r="AE26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AF26" s="17">
+      <c r="AF26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AG26" s="17">
+      <c r="AG26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AH26" s="17">
+      <c r="AH26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AI26" s="17">
+      <c r="AI26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AJ26" s="17">
+      <c r="AJ26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AK26" s="17">
+      <c r="AK26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AL26" s="17">
+      <c r="AL26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AM26" s="17">
+      <c r="AM26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AN26" s="17">
+      <c r="AN26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AO26" s="17">
+      <c r="AO26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AP26" s="17">
+      <c r="AP26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AQ26" s="17">
+      <c r="AQ26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AR26" s="17">
+      <c r="AR26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AS26" s="17">
+      <c r="AS26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AT26" s="17">
+      <c r="AT26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AU26" s="17">
+      <c r="AU26" s="1">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AV26" s="18">
+      <c r="AV26" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2703,7 +2689,7 @@
     </row>
     <row r="27" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="19"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -2762,341 +2748,447 @@
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="16">
         <v>1.6</v>
       </c>
       <c r="C28" s="1">
-        <v>2</v>
+        <f>IF(C21 = "0",0,2)</f>
+        <v>0</v>
       </c>
       <c r="D28" s="1">
-        <v>2.5</v>
+        <f>IF(D21 = "0",0,2.5)</f>
+        <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>3</v>
+        <f>IF(E21 = "0",0,3)</f>
+        <v>0</v>
       </c>
       <c r="F28" s="1">
-        <v>4</v>
+        <f>IF(F21 = "0",0,4)</f>
+        <v>0</v>
       </c>
       <c r="G28" s="1">
-        <v>5</v>
+        <f>IF(G21 = "0",0,5)</f>
+        <v>0</v>
       </c>
       <c r="H28" s="1">
-        <v>6</v>
+        <f>IF(H21 = "0",0,6)</f>
+        <v>0</v>
       </c>
       <c r="I28" s="1">
+        <f>IF(I21 = "0",0,8)</f>
         <v>8</v>
       </c>
       <c r="J28" s="1">
-        <v>10</v>
+        <f>IF(J21 = "0",0,10)</f>
+        <v>0</v>
       </c>
       <c r="K28" s="1">
-        <v>12</v>
+        <f>IF(K21 = "0",0,12)</f>
+        <v>0</v>
       </c>
       <c r="L28" s="1">
-        <v>16</v>
+        <f>IF(L21 = "0",0,16)</f>
+        <v>0</v>
       </c>
       <c r="M28" s="1">
-        <v>20</v>
+        <f>IF(M21 = "0",0,20)</f>
+        <v>0</v>
       </c>
       <c r="N28" s="1">
-        <v>24</v>
+        <f>IF(N21 = "0",0,24)</f>
+        <v>0</v>
       </c>
       <c r="O28" s="1">
-        <v>30</v>
+        <f>IF(O21 = "0",0,30)</f>
+        <v>0</v>
       </c>
       <c r="P28" s="1">
-        <v>36</v>
+        <f>IF(P21 = "0",0,36)</f>
+        <v>0</v>
       </c>
       <c r="Q28" s="13">
-        <v>42</v>
+        <f>IF(Q21 = "0",0,42)</f>
+        <v>0</v>
       </c>
       <c r="R28" s="15">
-        <v>2</v>
+        <f>IF(R21 = "0",0,2)</f>
+        <v>0</v>
       </c>
       <c r="S28" s="1">
-        <v>3</v>
+        <f>IF(S21 = "0",0,3)</f>
+        <v>0</v>
       </c>
       <c r="T28" s="1">
-        <v>4</v>
+        <f>IF(T21 = "0",0,4)</f>
+        <v>0</v>
       </c>
       <c r="U28" s="1">
-        <v>4</v>
+        <f>IF(U21 = "0",0,4)</f>
+        <v>0</v>
       </c>
       <c r="V28" s="1">
-        <v>5</v>
+        <f>IF(V21 = "0",0,5)</f>
+        <v>0</v>
       </c>
       <c r="W28" s="1">
-        <v>5</v>
+        <f t="shared" ref="W28" si="7">IF(W21 = "0",0,5)</f>
+        <v>0</v>
       </c>
       <c r="X28" s="1">
-        <v>6</v>
+        <f>IF(X21 = "0",0,6)</f>
+        <v>0</v>
       </c>
       <c r="Y28" s="1">
-        <v>6</v>
+        <f t="shared" ref="Y28:Z28" si="8">IF(Y21 = "0",0,6)</f>
+        <v>0</v>
       </c>
       <c r="Z28" s="1">
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="AA28" s="1">
-        <v>8</v>
+        <f>IF(AA21 = "0",0,8)</f>
+        <v>0</v>
       </c>
       <c r="AB28" s="1">
-        <v>8</v>
+        <f t="shared" ref="AB28:AC28" si="9">IF(AB21 = "0",0,8)</f>
+        <v>0</v>
       </c>
       <c r="AC28" s="1">
-        <v>8</v>
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="AD28" s="1">
-        <v>10</v>
+        <f>IF(AD21 = "0",0,10)</f>
+        <v>0</v>
       </c>
       <c r="AE28" s="1">
-        <v>10</v>
+        <f t="shared" ref="AE28:AF28" si="10">IF(AE21 = "0",0,10)</f>
+        <v>0</v>
       </c>
       <c r="AF28" s="1">
-        <v>10</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="AG28" s="1">
-        <v>12</v>
+        <f>IF(AG21 = "0",0,12)</f>
+        <v>0</v>
       </c>
       <c r="AH28" s="1">
-        <v>12</v>
+        <f t="shared" ref="AH28:AI28" si="11">IF(AH21 = "0",0,12)</f>
+        <v>0</v>
       </c>
       <c r="AI28" s="1">
-        <v>12</v>
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
       <c r="AJ28" s="1">
-        <v>16</v>
+        <f>IF(AJ21 = "0",0,16)</f>
+        <v>0</v>
       </c>
       <c r="AK28" s="1">
-        <v>16</v>
+        <f t="shared" ref="AK28:AL28" si="12">IF(AK21 = "0",0,16)</f>
+        <v>0</v>
       </c>
       <c r="AL28" s="1">
-        <v>16</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="AM28" s="1">
-        <v>20</v>
+        <f>IF(AM21 = "0",0,20)</f>
+        <v>0</v>
       </c>
       <c r="AN28" s="1">
-        <v>20</v>
+        <f t="shared" ref="AN28" si="13">IF(AN21 = "0",0,20)</f>
+        <v>0</v>
       </c>
       <c r="AO28" s="1">
-        <v>24</v>
+        <f>IF(AO21 = "0",0,24)</f>
+        <v>0</v>
       </c>
       <c r="AP28" s="1">
-        <v>24</v>
+        <f t="shared" ref="AP28" si="14">IF(AP21 = "0",0,24)</f>
+        <v>0</v>
       </c>
       <c r="AQ28" s="1">
-        <v>30</v>
+        <f>IF(AQ21 = "0",0,30)</f>
+        <v>0</v>
       </c>
       <c r="AR28" s="1">
-        <v>30</v>
+        <f t="shared" ref="AR28" si="15">IF(AR21 = "0",0,30)</f>
+        <v>0</v>
       </c>
       <c r="AS28" s="1">
-        <v>36</v>
+        <f>IF(AS21 = "0",0,36)</f>
+        <v>0</v>
       </c>
       <c r="AT28" s="1">
-        <v>36</v>
+        <f t="shared" ref="AT28" si="16">IF(AT21 = "0",0,36)</f>
+        <v>0</v>
       </c>
       <c r="AU28" s="1">
-        <v>42</v>
+        <f>IF(AU21 = "0",0,42)</f>
+        <v>0</v>
       </c>
       <c r="AV28" s="5">
-        <v>42</v>
-      </c>
-      <c r="AW28" s="8">
-        <v>6.4</v>
+        <f>IF(AV21 = "0",0,42)</f>
+        <v>0</v>
+      </c>
+      <c r="AW28" s="6">
+        <f>IF(AW21 = "0",0,6.4)</f>
+        <v>0</v>
       </c>
       <c r="AX28" s="1">
-        <v>7.95</v>
+        <f>IF(AX21 = "0",0,7.95)</f>
+        <v>0</v>
       </c>
       <c r="AY28" s="1">
-        <v>12.7</v>
+        <f>IF(AY21 = "0",0,12.7)</f>
+        <v>0</v>
       </c>
       <c r="AZ28" s="1">
-        <v>19.05</v>
-      </c>
-      <c r="BA28" s="14">
-        <v>25.4</v>
+        <f>IF(AZ21 = "0",0,19.05)</f>
+        <v>0</v>
+      </c>
+      <c r="BA28" s="1">
+        <f>IF(BA21 = "0",0,25.4)</f>
+        <v>0</v>
       </c>
       <c r="BB28" s="1">
-        <v>31.75</v>
+        <f>IF(BB21 = "0",0,31.75)</f>
+        <v>0</v>
       </c>
       <c r="BC28" s="1">
-        <v>38.1</v>
+        <f>IF(BC21 = "0",0,38.1)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="16">
         <v>3</v>
       </c>
       <c r="C29" s="1">
-        <v>3.8</v>
+        <f>IF(C21 = "0",0,3.8)</f>
+        <v>0</v>
       </c>
       <c r="D29" s="1">
-        <v>4.5</v>
+        <f>IF(D21 = "0",0,4.5)</f>
+        <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>5.5</v>
+        <f>IF(E21 = "0",0,5.5)</f>
+        <v>0</v>
       </c>
       <c r="F29" s="1">
-        <v>7</v>
+        <f>IF(F21 = "0",0,7)</f>
+        <v>0</v>
       </c>
       <c r="G29" s="1">
-        <v>8.5</v>
+        <f>IF(G21 = "0",0,8.5)</f>
+        <v>0</v>
       </c>
       <c r="H29" s="1">
-        <v>10</v>
+        <f>IF(H21 = "0",0,10)</f>
+        <v>0</v>
       </c>
       <c r="I29" s="1">
+        <f>IF(I21 = "0",0,13)</f>
         <v>13</v>
       </c>
       <c r="J29" s="1">
-        <v>16</v>
+        <f>IF(J21 = "0",0,16)</f>
+        <v>0</v>
       </c>
       <c r="K29" s="1">
-        <v>18</v>
+        <f>IF(K21 = "0",0,18)</f>
+        <v>0</v>
       </c>
       <c r="L29" s="1">
-        <v>24</v>
+        <f>IF(L21 = "0",0,24)</f>
+        <v>0</v>
       </c>
       <c r="M29" s="1">
-        <v>30</v>
+        <f>IF(M21 = "0",0,30)</f>
+        <v>0</v>
       </c>
       <c r="N29" s="1">
-        <v>36</v>
+        <f>IF(N21 = "0",0,36)</f>
+        <v>0</v>
       </c>
       <c r="O29" s="1">
-        <v>45</v>
+        <f>IF(O21 = "0",0,45)</f>
+        <v>0</v>
       </c>
       <c r="P29" s="1">
-        <v>54</v>
+        <f>IF(P21 = "0",0,54)</f>
+        <v>0</v>
       </c>
       <c r="Q29" s="13">
-        <v>63</v>
+        <f>IF(Q21 = "0",0,63)</f>
+        <v>0</v>
       </c>
       <c r="R29" s="15">
-        <v>3.8</v>
+        <f>IF(R21 = "0",0,3.8)</f>
+        <v>0</v>
       </c>
       <c r="S29" s="1">
-        <v>5.5</v>
+        <f>IF(S21 = "0",0,5.5)</f>
+        <v>0</v>
       </c>
       <c r="T29" s="1">
-        <v>7</v>
+        <f>IF(T21 = "0",0,7)</f>
+        <v>0</v>
       </c>
       <c r="U29" s="1">
-        <v>7</v>
+        <f t="shared" ref="U29" si="17">IF(U21 = "0",0,7)</f>
+        <v>0</v>
       </c>
       <c r="V29" s="1">
-        <v>8.5</v>
+        <f>IF(V21 = "0",0,8.5)</f>
+        <v>0</v>
       </c>
       <c r="W29" s="1">
-        <v>8.5</v>
+        <f t="shared" ref="W29" si="18">IF(W21 = "0",0,8.5)</f>
+        <v>0</v>
       </c>
       <c r="X29" s="1">
-        <v>10</v>
+        <f>IF(X21 = "0",0,10)</f>
+        <v>0</v>
       </c>
       <c r="Y29" s="1">
-        <v>10</v>
+        <f t="shared" ref="Y29:Z29" si="19">IF(Y21 = "0",0,10)</f>
+        <v>0</v>
       </c>
       <c r="Z29" s="1">
-        <v>10</v>
+        <f t="shared" si="19"/>
+        <v>0</v>
       </c>
       <c r="AA29" s="1">
-        <v>13</v>
+        <f>IF(AA21 = "0",0,13)</f>
+        <v>0</v>
       </c>
       <c r="AB29" s="1">
-        <v>13</v>
+        <f t="shared" ref="AB29:AC29" si="20">IF(AB21 = "0",0,13)</f>
+        <v>0</v>
       </c>
       <c r="AC29" s="1">
-        <v>13</v>
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
       <c r="AD29" s="1">
-        <v>16</v>
+        <f>IF(AD21 = "0",0,16)</f>
+        <v>0</v>
       </c>
       <c r="AE29" s="1">
-        <v>16</v>
+        <f t="shared" ref="AE29:AF29" si="21">IF(AE21 = "0",0,16)</f>
+        <v>0</v>
       </c>
       <c r="AF29" s="1">
-        <v>16</v>
+        <f t="shared" si="21"/>
+        <v>0</v>
       </c>
       <c r="AG29" s="1">
-        <v>18</v>
+        <f>IF(AG21 = "0",0,18)</f>
+        <v>0</v>
       </c>
       <c r="AH29" s="1">
-        <v>18</v>
+        <f t="shared" ref="AH29:AI29" si="22">IF(AH21 = "0",0,18)</f>
+        <v>0</v>
       </c>
       <c r="AI29" s="1">
-        <v>18</v>
+        <f t="shared" si="22"/>
+        <v>0</v>
       </c>
       <c r="AJ29" s="1">
-        <v>24</v>
+        <f>IF(AJ21 = "0",0,24)</f>
+        <v>0</v>
       </c>
       <c r="AK29" s="1">
-        <v>24</v>
+        <f t="shared" ref="AK29:AL29" si="23">IF(AK21 = "0",0,24)</f>
+        <v>0</v>
       </c>
       <c r="AL29" s="1">
-        <v>24</v>
+        <f t="shared" si="23"/>
+        <v>0</v>
       </c>
       <c r="AM29" s="1">
-        <v>30</v>
+        <f>IF(AM21 = "0",0,30)</f>
+        <v>0</v>
       </c>
       <c r="AN29" s="1">
-        <v>30</v>
+        <f t="shared" ref="AN29" si="24">IF(AN21 = "0",0,30)</f>
+        <v>0</v>
       </c>
       <c r="AO29" s="1">
-        <v>36</v>
+        <f>IF(AO21 = "0",0,36)</f>
+        <v>0</v>
       </c>
       <c r="AP29" s="1">
-        <v>36</v>
+        <f t="shared" ref="AP29" si="25">IF(AP21 = "0",0,36)</f>
+        <v>0</v>
       </c>
       <c r="AQ29" s="1">
-        <v>45</v>
+        <f>IF(AQ21 = "0",0,45)</f>
+        <v>0</v>
       </c>
       <c r="AR29" s="1">
-        <v>45</v>
+        <f t="shared" ref="AR29" si="26">IF(AR21 = "0",0,45)</f>
+        <v>0</v>
       </c>
       <c r="AS29" s="1">
-        <v>54</v>
+        <f>IF(AS21 = "0",0,54)</f>
+        <v>0</v>
       </c>
       <c r="AT29" s="1">
-        <v>54</v>
+        <f t="shared" ref="AT29" si="27">IF(AT21 = "0",0,54)</f>
+        <v>0</v>
       </c>
       <c r="AU29" s="1">
-        <v>63</v>
+        <f>IF(AU21 = "0",0,63)</f>
+        <v>0</v>
       </c>
       <c r="AV29" s="5">
-        <v>63</v>
-      </c>
-      <c r="AW29" s="8">
-        <v>7.95</v>
+        <f>IF(AV21 = "0",0,63)</f>
+        <v>0</v>
+      </c>
+      <c r="AW29" s="6">
+        <f>IF(AW21 = "0",0,7.95)</f>
+        <v>0</v>
       </c>
       <c r="AX29" s="1">
-        <v>12.7</v>
+        <f>IF(AX21 = "0",0,12.7)</f>
+        <v>0</v>
       </c>
       <c r="AY29" s="1">
-        <v>19.05</v>
+        <f>IF(AY21 = "0",0,19.05)</f>
+        <v>0</v>
       </c>
       <c r="AZ29" s="1">
-        <v>25.4</v>
-      </c>
-      <c r="BA29" s="14">
-        <v>31.75</v>
+        <f>IF(AZ21 = "0",0,25.4)</f>
+        <v>0</v>
+      </c>
+      <c r="BA29" s="1">
+        <f>IF(BA21 = "0",0,31.75)</f>
+        <v>0</v>
       </c>
       <c r="BB29" s="1">
-        <v>38.1</v>
+        <f>IF(BB21 = "0",0,38.1)</f>
+        <v>0</v>
       </c>
       <c r="BC29" s="1">
-        <v>44.45</v>
+        <f>IF(BC21 = "0",0,44.45)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="19">
+      <c r="B30" s="16">
         <f>IF(B21 ="1.6","1.5",0)</f>
         <v>0</v>
       </c>
@@ -3124,9 +3216,9 @@
         <f>IF(H21 ="6","5",0)</f>
         <v>0</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30" s="1" t="str">
         <f>IF(I21 ="8","6",0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J30" s="1">
         <f>IF(J21 ="10","8",0)</f>
@@ -3156,9 +3248,9 @@
         <f>IF(P21 ="36","27",0)</f>
         <v>0</v>
       </c>
-      <c r="Q30" s="13" t="str">
+      <c r="Q30" s="13">
         <f>IF(Q21 ="42","32",0)</f>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="R30" s="15">
         <f>IF(R21 ="2","1.5",0)</f>
@@ -3309,7 +3401,7 @@
         <v>0</v>
       </c>
       <c r="BC30" s="1" t="str">
-        <f t="shared" ref="BC30" si="7">IF(BC21 ="0","0","25.4")</f>
+        <f t="shared" ref="BC30" si="28">IF(BC21 ="0","0","25.4")</f>
         <v>0</v>
       </c>
     </row>
@@ -3317,220 +3409,220 @@
       <c r="A31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B31" s="16">
         <f>PI()/4*B29*B29 * B28 - ((6*(B30/COS(RADIANS(30)))*SIN(RADIANS(180/6))*B30)/4 * B28 *2/3)</f>
         <v>11.309733552923255</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" ref="C31:BA31" si="8">PI()/4*C29*C29 * C28 - ((6*(C30/COS(RADIANS(30)))*SIN(RADIANS(180/6))*C30)/4 * C28 *2/3)</f>
-        <v>22.682298958918306</v>
+        <f t="shared" ref="C31:BA31" si="29">PI()/4*C29*C29 * C28 - ((6*(C30/COS(RADIANS(30)))*SIN(RADIANS(180/6))*C30)/4 * C28 *2/3)</f>
+        <v>0</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="8"/>
-        <v>39.760782021995816</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="8"/>
-        <v>71.274883328318424</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="8"/>
-        <v>153.93804002589985</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="G31" s="1">
-        <f t="shared" si="8"/>
-        <v>283.72508652732824</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="8"/>
-        <v>471.23889803846896</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="8"/>
-        <v>1061.8583169133501</v>
+        <f t="shared" si="29"/>
+        <v>895.58143938673788</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="8"/>
-        <v>2010.6192982974676</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="8"/>
-        <v>3053.628059289279</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" si="8"/>
-        <v>7238.2294738708833</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="M31" s="1">
-        <f t="shared" si="8"/>
-        <v>14137.166941154068</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="N31" s="1">
-        <f t="shared" si="8"/>
-        <v>24429.024474314232</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="O31" s="1">
-        <f t="shared" si="8"/>
-        <v>47712.938426394991</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="P31" s="1">
-        <f t="shared" si="8"/>
-        <v>82447.957600810521</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="Q31" s="13">
-        <f t="shared" si="8"/>
-        <v>106093.62266472042</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="R31" s="15">
-        <f t="shared" si="8"/>
-        <v>22.682298958918306</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="S31" s="1">
-        <f t="shared" si="8"/>
-        <v>71.274883328318424</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="T31" s="1">
-        <f t="shared" si="8"/>
-        <v>153.93804002589985</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="U31" s="1">
-        <f t="shared" si="8"/>
-        <v>153.93804002589985</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="V31" s="1">
-        <f t="shared" si="8"/>
-        <v>283.72508652732824</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="W31" s="1">
-        <f t="shared" si="8"/>
-        <v>283.72508652732824</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="X31" s="1">
-        <f t="shared" si="8"/>
-        <v>471.23889803846896</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="Y31" s="1">
-        <f t="shared" si="8"/>
-        <v>471.23889803846896</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="Z31" s="1">
-        <f t="shared" si="8"/>
-        <v>471.23889803846896</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AA31" s="1">
-        <f t="shared" si="8"/>
-        <v>1061.8583169133501</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AB31" s="1">
-        <f t="shared" si="8"/>
-        <v>1061.8583169133501</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AC31" s="1">
-        <f t="shared" si="8"/>
-        <v>1061.8583169133501</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AD31" s="1">
-        <f t="shared" si="8"/>
-        <v>2010.6192982974676</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AE31" s="1">
-        <f t="shared" si="8"/>
-        <v>2010.6192982974676</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AF31" s="1">
-        <f t="shared" si="8"/>
-        <v>2010.6192982974676</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AG31" s="1">
-        <f t="shared" si="8"/>
-        <v>3053.628059289279</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AH31" s="1">
-        <f t="shared" si="8"/>
-        <v>3053.628059289279</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AI31" s="1">
-        <f t="shared" si="8"/>
-        <v>3053.628059289279</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AJ31" s="1">
-        <f t="shared" si="8"/>
-        <v>7238.2294738708833</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AK31" s="1">
-        <f t="shared" si="8"/>
-        <v>7238.2294738708833</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AL31" s="1">
-        <f t="shared" si="8"/>
-        <v>7238.2294738708833</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AM31" s="1">
-        <f t="shared" si="8"/>
-        <v>14137.166941154068</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AN31" s="1">
-        <f t="shared" si="8"/>
-        <v>14137.166941154068</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AO31" s="1">
-        <f t="shared" si="8"/>
-        <v>24429.024474314232</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AP31" s="1">
-        <f t="shared" si="8"/>
-        <v>24429.024474314232</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AQ31" s="1">
-        <f t="shared" si="8"/>
-        <v>47712.938426394991</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AR31" s="1">
-        <f t="shared" si="8"/>
-        <v>47712.938426394991</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AS31" s="1">
-        <f t="shared" si="8"/>
-        <v>82447.957600810521</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AT31" s="1">
-        <f t="shared" si="8"/>
-        <v>82447.957600810521</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AU31" s="1">
-        <f t="shared" si="8"/>
-        <v>130924.30304202784</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AV31" s="5">
-        <f t="shared" si="8"/>
-        <v>130924.30304202784</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AW31" s="6">
-        <f t="shared" si="8"/>
-        <v>317.69041550161427</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AX31" s="1">
-        <f t="shared" si="8"/>
-        <v>1007.0811147062767</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AY31" s="1">
-        <f t="shared" si="8"/>
-        <v>3619.7915538027501</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="AZ31" s="1">
-        <f t="shared" si="8"/>
-        <v>9652.7774768073323</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="BA31" s="1">
-        <f t="shared" si="8"/>
-        <v>20109.953076681941</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="BB31" s="1"/>
       <c r="BC31" s="1"/>
     </row>
     <row r="32" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="19"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -3589,174 +3681,227 @@
       <c r="A33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="19">
+      <c r="B33" s="16">
         <v>1.1000000000000001</v>
       </c>
       <c r="C33" s="1">
-        <v>1.4</v>
+        <f>IF(C21= "0",0,1.4)</f>
+        <v>0</v>
       </c>
       <c r="D33" s="1">
-        <v>1.7</v>
+        <f>IF(D21= "0",0,1.7)</f>
+        <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>2</v>
+        <f>IF(E21= "0",0,2)</f>
+        <v>0</v>
       </c>
       <c r="F33" s="1">
-        <v>2.8</v>
+        <f>IF(F21= "0",0,2.8)</f>
+        <v>0</v>
       </c>
       <c r="G33" s="1">
-        <v>3.5</v>
+        <f>IF(G21= "0",0,3.5)</f>
+        <v>0</v>
       </c>
       <c r="H33" s="1">
-        <v>4</v>
+        <f>IF(H21= "0",0,4)</f>
+        <v>0</v>
       </c>
       <c r="I33" s="1">
+        <f>IF(I21= "0",0,5.3)</f>
         <v>5.3</v>
       </c>
       <c r="J33" s="1">
-        <v>6.4</v>
+        <f>IF(J21= "0",0,6.4)</f>
+        <v>0</v>
       </c>
       <c r="K33" s="1">
-        <v>7.5</v>
+        <f>IF(K21= "0",0,7.5)</f>
+        <v>0</v>
       </c>
       <c r="L33" s="1">
-        <v>10</v>
+        <f>IF(L21= "0",0,10)</f>
+        <v>0</v>
       </c>
       <c r="M33" s="1">
-        <v>12.5</v>
+        <f>IF(M21= "0",0,12.5)</f>
+        <v>0</v>
       </c>
       <c r="N33" s="1">
-        <v>15</v>
+        <f>IF(N21= "0",0,15)</f>
+        <v>0</v>
       </c>
       <c r="O33" s="1">
-        <v>18.7</v>
+        <f>IF(O21= "0",0,18.7)</f>
+        <v>0</v>
       </c>
       <c r="P33" s="1">
-        <v>22.5</v>
+        <f>IF(P21= "0",0,22.5)</f>
+        <v>0</v>
       </c>
       <c r="Q33" s="13">
-        <v>26</v>
+        <f>IF(Q21= "0",0,26)</f>
+        <v>0</v>
       </c>
       <c r="R33" s="15">
-        <v>1.4</v>
+        <f>IF(R21= "0",0,1.4)</f>
+        <v>0</v>
       </c>
       <c r="S33" s="1">
-        <v>2</v>
+        <f>IF(S21= "0",0,2)</f>
+        <v>0</v>
       </c>
       <c r="T33" s="1">
-        <v>2.8</v>
+        <f>IF(T21= "0",0,2.8)</f>
+        <v>0</v>
       </c>
       <c r="U33" s="1">
-        <v>2.8</v>
+        <f t="shared" ref="U33:V33" si="30">IF(U21= "0",0,2.8)</f>
+        <v>0</v>
       </c>
       <c r="V33" s="1">
-        <v>3.5</v>
+        <f>IF(V21= "0",0,3.5)</f>
+        <v>0</v>
       </c>
       <c r="W33" s="1">
-        <v>3.5</v>
+        <f t="shared" ref="W33:X33" si="31">IF(W21= "0",0,3.5)</f>
+        <v>0</v>
       </c>
       <c r="X33" s="1">
-        <v>4</v>
+        <f>IF(X21= "0",0,4)</f>
+        <v>0</v>
       </c>
       <c r="Y33" s="1">
-        <v>4</v>
+        <f t="shared" ref="Y33:AA33" si="32">IF(Y21= "0",0,4)</f>
+        <v>0</v>
       </c>
       <c r="Z33" s="1">
-        <v>4</v>
+        <f t="shared" si="32"/>
+        <v>0</v>
       </c>
       <c r="AA33" s="1">
-        <v>5.3</v>
+        <f>IF(AA21= "0",0,5.3)</f>
+        <v>0</v>
       </c>
       <c r="AB33" s="1">
-        <v>5.3</v>
+        <f t="shared" ref="AB33:AD33" si="33">IF(AB21= "0",0,5.3)</f>
+        <v>0</v>
       </c>
       <c r="AC33" s="1">
-        <v>5.3</v>
+        <f t="shared" si="33"/>
+        <v>0</v>
       </c>
       <c r="AD33" s="1">
-        <v>6.4</v>
+        <f>IF(AD21= "0",0,6.4)</f>
+        <v>0</v>
       </c>
       <c r="AE33" s="1">
-        <v>6.4</v>
+        <f t="shared" ref="AE33:AF33" si="34">IF(AE21= "0",0,6.4)</f>
+        <v>0</v>
       </c>
       <c r="AF33" s="1">
-        <v>6.4</v>
+        <f t="shared" si="34"/>
+        <v>0</v>
       </c>
       <c r="AG33" s="1">
-        <v>7.5</v>
+        <f>IF(AG21= "0",0,7.5)</f>
+        <v>0</v>
       </c>
       <c r="AH33" s="1">
-        <v>7.5</v>
+        <f t="shared" ref="AH33:AJ33" si="35">IF(AH21= "0",0,7.5)</f>
+        <v>0</v>
       </c>
       <c r="AI33" s="1">
-        <v>7.5</v>
+        <f t="shared" si="35"/>
+        <v>0</v>
       </c>
       <c r="AJ33" s="1">
-        <v>10</v>
+        <f>IF(AJ21= "0",0,10)</f>
+        <v>0</v>
       </c>
       <c r="AK33" s="1">
-        <v>10</v>
+        <f t="shared" ref="AK33:AM33" si="36">IF(AK21= "0",0,10)</f>
+        <v>0</v>
       </c>
       <c r="AL33" s="1">
-        <v>10</v>
+        <f t="shared" si="36"/>
+        <v>0</v>
       </c>
       <c r="AM33" s="1">
-        <v>12.5</v>
+        <f>IF(AM21= "0",0,12.5)</f>
+        <v>0</v>
       </c>
       <c r="AN33" s="1">
-        <v>12.5</v>
+        <f t="shared" ref="AN33:AO33" si="37">IF(AN21= "0",0,12.5)</f>
+        <v>0</v>
       </c>
       <c r="AO33" s="1">
-        <v>15</v>
+        <f>IF(AO21= "0",0,15)</f>
+        <v>0</v>
       </c>
       <c r="AP33" s="1">
-        <v>15</v>
+        <f t="shared" ref="AP33:AQ33" si="38">IF(AP21= "0",0,15)</f>
+        <v>0</v>
       </c>
       <c r="AQ33" s="1">
-        <v>18.7</v>
+        <f>IF(AQ21= "0",0,18.7)</f>
+        <v>0</v>
       </c>
       <c r="AR33" s="1">
-        <v>18.7</v>
+        <f t="shared" ref="AR33:AS33" si="39">IF(AR21= "0",0,18.7)</f>
+        <v>0</v>
       </c>
       <c r="AS33" s="1">
-        <v>22.5</v>
+        <f>IF(AS21= "0",0,22.5)</f>
+        <v>0</v>
       </c>
       <c r="AT33" s="1">
-        <v>22.5</v>
+        <f t="shared" ref="AT33:AU33" si="40">IF(AT21= "0",0,22.5)</f>
+        <v>0</v>
       </c>
       <c r="AU33" s="1">
-        <v>26</v>
+        <f>IF(AU21= "0",0,26)</f>
+        <v>0</v>
       </c>
       <c r="AV33" s="5">
-        <v>26</v>
-      </c>
-      <c r="AW33" s="8">
-        <v>4</v>
+        <f>IF(AV21= "0",0,26)</f>
+        <v>0</v>
+      </c>
+      <c r="AW33" s="6">
+        <f>IF(AW21= "0",0,4)</f>
+        <v>0</v>
       </c>
       <c r="AX33" s="1">
-        <v>6</v>
+        <f>IF(AX21= "0",0,6)</f>
+        <v>0</v>
       </c>
       <c r="AY33" s="1">
-        <v>7.95</v>
+        <f>IF(AY21= "0",0,7.95)</f>
+        <v>0</v>
       </c>
       <c r="AZ33" s="1">
-        <v>11.9</v>
-      </c>
-      <c r="BA33" s="14">
-        <v>15.5</v>
-      </c>
-      <c r="BB33" s="14">
-        <v>19.8</v>
-      </c>
-      <c r="BC33" s="14">
-        <v>23.8</v>
+        <f>IF(AZ21= "0",0,11.9)</f>
+        <v>0</v>
+      </c>
+      <c r="BA33" s="1">
+        <f>IF(BA21= "0",0,15.5)</f>
+        <v>0</v>
+      </c>
+      <c r="BB33" s="1">
+        <f>IF(BB21= "0",0,19.8)</f>
+        <v>0</v>
+      </c>
+      <c r="BC33" s="1">
+        <f>IF(BC21= "0",0,23.8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="19">
+      <c r="B34" s="16">
         <f>IF(B21 ="1.6","3.2",0)</f>
         <v>0</v>
       </c>
@@ -3784,9 +3929,9 @@
         <f>IF(H21 ="6","10",0)</f>
         <v>0</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I34" s="1" t="str">
         <f>IF(I21 ="8","13",0)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J34" s="1">
         <f>IF(J21 ="10","17",0)</f>
@@ -3816,9 +3961,9 @@
         <f>IF(P21 ="36","55",0)</f>
         <v>0</v>
       </c>
-      <c r="Q34" s="13" t="str">
+      <c r="Q34" s="13">
         <f>IF(Q21 ="42","65",0)</f>
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="R34" s="15">
         <f>IF(R21 ="2","4",0)</f>
@@ -3977,16 +4122,16 @@
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="19">
-        <f t="shared" ref="B35:D35" si="9">((6*(B34/COS(RADIANS(30)))*SIN(RADIANS(180/6))*B34)/4) *B33</f>
+      <c r="B35" s="16">
+        <f t="shared" ref="B35:D35" si="41">((6*(B34/COS(RADIANS(30)))*SIN(RADIANS(180/6))*B34)/4) *B33</f>
         <v>0</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="E35" s="1">
@@ -3994,209 +4139,209 @@
         <v>0</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" ref="F35:BC35" si="10">((6*(F34/COS(RADIANS(30)))*SIN(RADIANS(180/6))*F34)/4) *F33</f>
+        <f t="shared" ref="F35:BC35" si="42">((6*(F34/COS(RADIANS(30)))*SIN(RADIANS(180/6))*F34)/4) *F33</f>
         <v>0</v>
       </c>
       <c r="G35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="42"/>
+        <v>775.69895416972145</v>
       </c>
       <c r="J35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="L35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="M35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="N35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="O35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="Q35" s="13">
-        <f t="shared" si="10"/>
-        <v>95132.89060572056</v>
+        <f t="shared" si="42"/>
+        <v>0</v>
       </c>
       <c r="R35" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="S35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="T35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="U35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="V35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="W35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="X35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="Y35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="Z35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AA35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AB35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AC35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AD35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AE35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AF35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AG35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AH35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AI35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AJ35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AK35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AL35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AM35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AN35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AO35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AP35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AQ35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AR35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AS35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AT35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AU35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AV35" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AW35" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AX35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AY35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="AZ35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="BA35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="BB35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="BC35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="19"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -4255,114 +4400,148 @@
       <c r="A37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="16"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1">
-        <v>1.9</v>
+        <f>IF(E21 ="0",0,1.9)</f>
+        <v>0</v>
       </c>
       <c r="F37" s="1">
-        <v>2.5</v>
+        <f>IF(F21 ="0",0,2.5)</f>
+        <v>0</v>
       </c>
       <c r="G37" s="1">
-        <v>3.1</v>
+        <f>IF(G21 ="0",0,3.1)</f>
+        <v>0</v>
       </c>
       <c r="H37" s="1">
-        <v>3.7</v>
+        <f>IF(H21 ="0",0,3.7)</f>
+        <v>0</v>
       </c>
       <c r="I37" s="1">
+        <f>IF(I21 ="0",0,5)</f>
         <v>5</v>
       </c>
       <c r="J37" s="1">
-        <v>6.2</v>
+        <f>IF(J21 ="0",0,6.2)</f>
+        <v>0</v>
       </c>
       <c r="K37" s="1">
-        <v>7.4</v>
+        <f>IF(K21 ="0",0,7.4)</f>
+        <v>0</v>
       </c>
       <c r="L37" s="1">
-        <v>8.8000000000000007</v>
+        <f>IF(L21 ="0",0,8.8)</f>
+        <v>0</v>
       </c>
       <c r="M37" s="1">
-        <v>10.199999999999999</v>
+        <f>IF(M21 ="0",0,10.2)</f>
+        <v>0</v>
       </c>
       <c r="N37" s="1">
-        <v>14</v>
+        <f>IF(N21 ="0",0,14)</f>
+        <v>0</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="13"/>
       <c r="R37" s="15"/>
       <c r="S37" s="1">
-        <v>1.9</v>
+        <f>IF(S21 ="0",0,1.9)</f>
+        <v>0</v>
       </c>
       <c r="T37" s="1">
-        <v>2.5</v>
+        <f>IF(T21 ="0",0,2.5)</f>
+        <v>0</v>
       </c>
       <c r="U37" s="1">
-        <v>2.5</v>
+        <f t="shared" ref="U37" si="43">IF(U21 ="0",0,2.5)</f>
+        <v>0</v>
       </c>
       <c r="V37" s="1">
-        <v>3.1</v>
+        <f>IF(V21 ="0",0,3.1)</f>
+        <v>0</v>
       </c>
       <c r="W37" s="1">
-        <v>3.1</v>
+        <f t="shared" ref="W37" si="44">IF(W21 ="0",0,3.1)</f>
+        <v>0</v>
       </c>
       <c r="X37" s="1">
-        <v>3.7</v>
+        <f>IF(X21 ="0",0,3.7)</f>
+        <v>0</v>
       </c>
       <c r="Y37" s="1">
-        <v>3.7</v>
+        <f t="shared" ref="Y37:Z37" si="45">IF(Y21 ="0",0,3.7)</f>
+        <v>0</v>
       </c>
       <c r="Z37" s="1">
-        <v>5</v>
+        <f t="shared" si="45"/>
+        <v>0</v>
       </c>
       <c r="AA37" s="1">
-        <v>5</v>
+        <f>IF(AA21 ="0",0,5)</f>
+        <v>0</v>
       </c>
       <c r="AB37" s="1">
-        <v>5</v>
+        <f t="shared" ref="AB37:AC37" si="46">IF(AB21 ="0",0,5)</f>
+        <v>0</v>
       </c>
       <c r="AC37" s="1">
-        <v>5</v>
+        <f t="shared" si="46"/>
+        <v>0</v>
       </c>
       <c r="AD37" s="1">
-        <v>6.2</v>
+        <f>IF(AD21 ="0",0,6.2)</f>
+        <v>0</v>
       </c>
       <c r="AE37" s="1">
-        <v>6.2</v>
+        <f t="shared" ref="AE37:AF37" si="47">IF(AE21 ="0",0,6.2)</f>
+        <v>0</v>
       </c>
       <c r="AF37" s="1">
-        <v>6.2</v>
+        <f t="shared" si="47"/>
+        <v>0</v>
       </c>
       <c r="AG37" s="1">
-        <v>7.4</v>
+        <f>IF(AG21 ="0",0,7.4)</f>
+        <v>0</v>
       </c>
       <c r="AH37" s="1">
-        <v>7.4</v>
+        <f t="shared" ref="AH37:AI37" si="48">IF(AH21 ="0",0,7.4)</f>
+        <v>0</v>
       </c>
       <c r="AI37" s="1">
-        <v>7.4</v>
+        <f t="shared" si="48"/>
+        <v>0</v>
       </c>
       <c r="AJ37" s="1">
-        <v>8.8000000000000007</v>
+        <f>IF(AJ21 ="0",0,8.8)</f>
+        <v>0</v>
       </c>
       <c r="AK37" s="1">
-        <v>8.8000000000000007</v>
+        <f t="shared" ref="AK37:AL37" si="49">IF(AK21 ="0",0,8.8)</f>
+        <v>0</v>
       </c>
       <c r="AL37" s="1">
-        <v>8.8000000000000007</v>
+        <f t="shared" si="49"/>
+        <v>0</v>
       </c>
       <c r="AM37" s="1">
-        <v>10.199999999999999</v>
+        <f>IF(AM21 ="0",0,10.2)</f>
+        <v>0</v>
       </c>
       <c r="AN37" s="1">
-        <v>10.199999999999999</v>
+        <f t="shared" ref="AN37" si="50">IF(AN21 ="0",0,10.2)</f>
+        <v>0</v>
       </c>
       <c r="AO37" s="1">
-        <v>14</v>
+        <f>IF(AO21 ="0",0,14)</f>
+        <v>0</v>
       </c>
       <c r="AP37" s="1">
-        <v>14</v>
+        <f>IF(AP21 ="0",0,14)</f>
+        <v>0</v>
       </c>
       <c r="AQ37" s="1"/>
       <c r="AR37" s="1"/>
@@ -4370,14 +4549,17 @@
       <c r="AT37" s="1"/>
       <c r="AU37" s="1"/>
       <c r="AV37" s="5"/>
-      <c r="AW37" s="8">
-        <v>4.0999999999999996</v>
+      <c r="AW37" s="6">
+        <f>IF(AW21 ="0",0,4.1)</f>
+        <v>0</v>
       </c>
       <c r="AX37" s="1">
-        <v>5.9</v>
+        <f>IF(AX21 ="0",0,5.9)</f>
+        <v>0</v>
       </c>
       <c r="AY37" s="1">
-        <v>6.4</v>
+        <f>IF(AY21 ="0",0,6.4)</f>
+        <v>0</v>
       </c>
       <c r="AZ37" s="1"/>
       <c r="BA37" s="1"/>
@@ -4388,114 +4570,148 @@
       <c r="A38" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="19"/>
+      <c r="B38" s="16"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1">
-        <v>5.5</v>
+        <f>IF(E21 ="0",0,5.5)</f>
+        <v>0</v>
       </c>
       <c r="F38" s="1">
-        <v>7.5</v>
+        <f>IF(F21 ="0",0,7.5)</f>
+        <v>0</v>
       </c>
       <c r="G38" s="1">
-        <v>9.4</v>
+        <f>IF(G21 ="0",0,9.4)</f>
+        <v>0</v>
       </c>
       <c r="H38" s="1">
-        <v>11.3</v>
+        <f>IF(H21 ="0",0,11.3)</f>
+        <v>0</v>
       </c>
       <c r="I38" s="1">
+        <f>IF(I21 ="0",0,15.2)</f>
         <v>15.2</v>
       </c>
       <c r="J38" s="1">
-        <v>19.2</v>
+        <f>IF(J21 ="0",0,19.2)</f>
+        <v>0</v>
       </c>
       <c r="K38" s="1">
-        <v>23.1</v>
+        <f>IF(K21 ="0",0,23.1)</f>
+        <v>0</v>
       </c>
       <c r="L38" s="1">
-        <v>29</v>
+        <f>IF(L21 ="0",0,29)</f>
+        <v>0</v>
       </c>
       <c r="M38" s="1">
-        <v>36</v>
+        <f>IF(M21 ="0",0,36)</f>
+        <v>0</v>
       </c>
       <c r="N38" s="1">
-        <v>39</v>
+        <f>IF(N21 ="0",0,39)</f>
+        <v>0</v>
       </c>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="13"/>
       <c r="R38" s="15"/>
       <c r="S38" s="1">
-        <v>5.5</v>
+        <f>IF(S21 ="0",0,5.5)</f>
+        <v>0</v>
       </c>
       <c r="T38" s="1">
-        <v>7.5</v>
+        <f>IF(T21 ="0",0,7.5)</f>
+        <v>0</v>
       </c>
       <c r="U38" s="1">
-        <v>7.5</v>
+        <f t="shared" ref="U38" si="51">IF(U21 ="0",0,7.5)</f>
+        <v>0</v>
       </c>
       <c r="V38" s="1">
-        <v>9.4</v>
+        <f>IF(V21 ="0",0,9.4)</f>
+        <v>0</v>
       </c>
       <c r="W38" s="1">
-        <v>9.4</v>
+        <f t="shared" ref="W38" si="52">IF(W21 ="0",0,9.4)</f>
+        <v>0</v>
       </c>
       <c r="X38" s="1">
-        <v>11.3</v>
+        <f>IF(X21 ="0",0,11.3)</f>
+        <v>0</v>
       </c>
       <c r="Y38" s="1">
-        <v>11.3</v>
+        <f t="shared" ref="Y38:Z38" si="53">IF(Y21 ="0",0,11.3)</f>
+        <v>0</v>
       </c>
       <c r="Z38" s="1">
-        <v>15.2</v>
+        <f t="shared" si="53"/>
+        <v>0</v>
       </c>
       <c r="AA38" s="1">
-        <v>15.2</v>
+        <f>IF(AA21 ="0",0,15.2)</f>
+        <v>0</v>
       </c>
       <c r="AB38" s="1">
-        <v>15.2</v>
+        <f t="shared" ref="AB38:AC38" si="54">IF(AB21 ="0",0,15.2)</f>
+        <v>0</v>
       </c>
       <c r="AC38" s="1">
-        <v>15.2</v>
+        <f t="shared" si="54"/>
+        <v>0</v>
       </c>
       <c r="AD38" s="1">
-        <v>19.2</v>
+        <f>IF(AD21 ="0",0,19.2)</f>
+        <v>0</v>
       </c>
       <c r="AE38" s="1">
-        <v>19.2</v>
+        <f t="shared" ref="AE38:AF38" si="55">IF(AE21 ="0",0,19.2)</f>
+        <v>0</v>
       </c>
       <c r="AF38" s="1">
-        <v>19.2</v>
+        <f t="shared" si="55"/>
+        <v>0</v>
       </c>
       <c r="AG38" s="1">
-        <v>23.1</v>
+        <f>IF(AG21 ="0",0,23.1)</f>
+        <v>0</v>
       </c>
       <c r="AH38" s="1">
-        <v>23.1</v>
+        <f t="shared" ref="AH38:AI38" si="56">IF(AH21 ="0",0,23.1)</f>
+        <v>0</v>
       </c>
       <c r="AI38" s="1">
-        <v>23.1</v>
+        <f t="shared" si="56"/>
+        <v>0</v>
       </c>
       <c r="AJ38" s="1">
-        <v>29</v>
+        <f>IF(AJ21 ="0",0,29)</f>
+        <v>0</v>
       </c>
       <c r="AK38" s="1">
-        <v>29</v>
+        <f t="shared" ref="AK38:AL38" si="57">IF(AK21 ="0",0,29)</f>
+        <v>0</v>
       </c>
       <c r="AL38" s="1">
-        <v>29</v>
+        <f t="shared" si="57"/>
+        <v>0</v>
       </c>
       <c r="AM38" s="1">
-        <v>36</v>
+        <f>IF(AM21 ="0",0,36)</f>
+        <v>0</v>
       </c>
       <c r="AN38" s="1">
-        <v>36</v>
+        <f t="shared" ref="AN38" si="58">IF(AN21 ="0",0,36)</f>
+        <v>0</v>
       </c>
       <c r="AO38" s="1">
-        <v>39</v>
+        <f>IF(AO21 ="0",0,39)</f>
+        <v>0</v>
       </c>
       <c r="AP38" s="1">
-        <v>39</v>
+        <f>IF(AP21 ="0",0,39)</f>
+        <v>0</v>
       </c>
       <c r="AQ38" s="1"/>
       <c r="AR38" s="1"/>
@@ -4503,14 +4719,17 @@
       <c r="AT38" s="1"/>
       <c r="AU38" s="1"/>
       <c r="AV38" s="5"/>
-      <c r="AW38" s="8">
-        <v>12.7</v>
+      <c r="AW38" s="6">
+        <f>IF(AW21 ="0",0,12.7)</f>
+        <v>0</v>
       </c>
       <c r="AX38" s="1">
-        <v>19</v>
+        <f>IF(AX21 ="0",0,19)</f>
+        <v>0</v>
       </c>
       <c r="AY38" s="1">
-        <v>25.4</v>
+        <f>IF(AY21 ="0",0,25.4)</f>
+        <v>0</v>
       </c>
       <c r="AZ38" s="1"/>
       <c r="BA38" s="1"/>
@@ -4521,7 +4740,7 @@
       <c r="A39" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="19"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1">
@@ -4540,9 +4759,9 @@
         <f>IF(H21 ="6","4",0)</f>
         <v>0</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I39" s="1" t="str">
         <f>IF(I21 ="8","5",0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J39" s="1">
         <f>IF(J21 ="10","6",0)</f>
@@ -4679,7 +4898,7 @@
         <v>0</v>
       </c>
       <c r="AY39" s="1" t="str">
-        <f t="shared" ref="AY39" si="11">IF(AY21="0","0","7.95")</f>
+        <f t="shared" ref="AY39" si="59">IF(AY21="0","0","7.95")</f>
         <v>0</v>
       </c>
       <c r="AZ39" s="1"/>
@@ -4691,148 +4910,148 @@
       <c r="A40" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="19"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1">
         <f>PI()/4*E38*E38 * E37 * 0.5  - ((6*(E39/COS(RADIANS(30)))*SIN(RADIANS(180/6))*E39)/4 * E37 *2/3)</f>
-        <v>22.570379720634168</v>
+        <v>0</v>
       </c>
       <c r="F40" s="1">
-        <f t="shared" ref="F40:N40" si="12">PI()/4*F38*F38 * F37 * 0.5  - ((6*(F39/COS(RADIANS(30)))*SIN(RADIANS(180/6))*F39)/4 * F37 *2/3)</f>
-        <v>55.223308363883078</v>
+        <f t="shared" ref="F40:N40" si="60">PI()/4*F38*F38 * F37 * 0.5  - ((6*(F39/COS(RADIANS(30)))*SIN(RADIANS(180/6))*F39)/4 * F37 *2/3)</f>
+        <v>0</v>
       </c>
       <c r="G40" s="1">
-        <f t="shared" si="12"/>
-        <v>107.56656166258773</v>
+        <f t="shared" si="60"/>
+        <v>0</v>
       </c>
       <c r="H40" s="1">
-        <f t="shared" si="12"/>
-        <v>185.53185924580734</v>
+        <f t="shared" si="60"/>
+        <v>0</v>
       </c>
       <c r="I40" s="1">
-        <f t="shared" si="12"/>
-        <v>453.64597917836613</v>
+        <f t="shared" si="60"/>
+        <v>381.47719552966294</v>
       </c>
       <c r="J40" s="1">
-        <f t="shared" si="12"/>
-        <v>897.54045475998964</v>
+        <f t="shared" si="60"/>
+        <v>0</v>
       </c>
       <c r="K40" s="1">
-        <f t="shared" si="12"/>
-        <v>1550.6563616908959</v>
+        <f t="shared" si="60"/>
+        <v>0</v>
       </c>
       <c r="L40" s="1">
-        <f t="shared" si="12"/>
-        <v>2906.2873638359179</v>
+        <f t="shared" si="60"/>
+        <v>0</v>
       </c>
       <c r="M40" s="1">
-        <f t="shared" si="12"/>
-        <v>5191.1677007917733</v>
+        <f t="shared" si="60"/>
+        <v>0</v>
       </c>
       <c r="N40" s="1">
-        <f t="shared" si="12"/>
-        <v>8362.1342456926304</v>
+        <f t="shared" si="60"/>
+        <v>0</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="13"/>
       <c r="R40" s="15"/>
       <c r="S40" s="1">
-        <f t="shared" ref="S40:AP40" si="13">PI()/4*S38*S38 * S37 * 0.5  - ((6*(S39/COS(RADIANS(30)))*SIN(RADIANS(180/6))*S39)/4 * S37 *2/3)</f>
-        <v>22.570379720634168</v>
+        <f t="shared" ref="S40:AP40" si="61">PI()/4*S38*S38 * S37 * 0.5  - ((6*(S39/COS(RADIANS(30)))*SIN(RADIANS(180/6))*S39)/4 * S37 *2/3)</f>
+        <v>0</v>
       </c>
       <c r="T40" s="1">
-        <f t="shared" si="13"/>
-        <v>55.223308363883078</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="U40" s="1">
-        <f t="shared" si="13"/>
-        <v>55.223308363883078</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="V40" s="1">
-        <f t="shared" si="13"/>
-        <v>107.56656166258773</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="W40" s="1">
-        <f t="shared" si="13"/>
-        <v>107.56656166258773</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="X40" s="1">
-        <f t="shared" si="13"/>
-        <v>185.53185924580734</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="Y40" s="1">
-        <f t="shared" si="13"/>
-        <v>185.53185924580734</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="Z40" s="1">
-        <f t="shared" si="13"/>
-        <v>453.64597917836613</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AA40" s="1">
-        <f t="shared" si="13"/>
-        <v>453.64597917836613</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AB40" s="1">
-        <f t="shared" si="13"/>
-        <v>453.64597917836613</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AC40" s="1">
-        <f t="shared" si="13"/>
-        <v>453.64597917836613</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AD40" s="1">
-        <f t="shared" si="13"/>
-        <v>897.54045475998964</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AE40" s="1">
-        <f t="shared" si="13"/>
-        <v>897.54045475998964</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AF40" s="1">
-        <f t="shared" si="13"/>
-        <v>897.54045475998964</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AG40" s="1">
-        <f t="shared" si="13"/>
-        <v>1550.6563616908959</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AH40" s="1">
-        <f t="shared" si="13"/>
-        <v>1550.6563616908959</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AI40" s="1">
-        <f t="shared" si="13"/>
-        <v>1550.6563616908959</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AJ40" s="1">
-        <f t="shared" si="13"/>
-        <v>2906.2873638359179</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AK40" s="1">
-        <f t="shared" si="13"/>
-        <v>2906.2873638359179</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AL40" s="1">
-        <f t="shared" si="13"/>
-        <v>2906.2873638359179</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AM40" s="1">
-        <f t="shared" si="13"/>
-        <v>5191.1677007917733</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AN40" s="1">
-        <f t="shared" si="13"/>
-        <v>5191.1677007917733</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AO40" s="1">
-        <f t="shared" si="13"/>
-        <v>8362.1342456926304</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AP40" s="1">
-        <f t="shared" si="13"/>
-        <v>8362.1342456926304</v>
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
       <c r="AQ40" s="1"/>
       <c r="AR40" s="1"/>
@@ -4841,16 +5060,16 @@
       <c r="AU40" s="1"/>
       <c r="AV40" s="5"/>
       <c r="AW40" s="6">
-        <f t="shared" ref="AW40:AY40" si="14">PI()/4*AW38*AW38 * AW37 * 0.5  - ((6*(AW39/COS(RADIANS(30)))*SIN(RADIANS(180/6))*AW39)/4 * AW37 *2/3)</f>
-        <v>259.68758303746756</v>
+        <f t="shared" ref="AW40:AY40" si="62">PI()/4*AW38*AW38 * AW37 * 0.5  - ((6*(AW39/COS(RADIANS(30)))*SIN(RADIANS(180/6))*AW39)/4 * AW37 *2/3)</f>
+        <v>0</v>
       </c>
       <c r="AX40" s="1">
-        <f t="shared" si="14"/>
-        <v>836.40977411011249</v>
+        <f t="shared" si="62"/>
+        <v>0</v>
       </c>
       <c r="AY40" s="1">
-        <f t="shared" si="14"/>
-        <v>1621.4639331119927</v>
+        <f t="shared" si="62"/>
+        <v>0</v>
       </c>
       <c r="AZ40" s="1"/>
       <c r="BA40" s="1"/>
@@ -4861,220 +5080,220 @@
       <c r="A41" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="19">
-        <f t="shared" ref="B41:BC41" si="15">PI()/4*B21*B21*$B9</f>
+      <c r="B41" s="16">
+        <f t="shared" ref="B41:BC41" si="63">PI()/4*B21*B21*$B9</f>
         <v>0</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="D41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="F41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="G41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="H41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="I41" s="1">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f t="shared" si="63"/>
+        <v>50265.482457436687</v>
       </c>
       <c r="J41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="K41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="L41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="M41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="N41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="O41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="P41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="Q41" s="13">
-        <f t="shared" si="15"/>
-        <v>1385442.360233099</v>
+        <f t="shared" si="63"/>
+        <v>0</v>
       </c>
       <c r="R41" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="S41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="T41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="U41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="V41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="W41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="X41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="Y41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="Z41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AA41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AB41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AC41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AD41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AE41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AF41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AG41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AH41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AI41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AJ41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AK41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AL41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AM41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AN41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AO41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AP41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AQ41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AR41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AS41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AT41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AU41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AV41" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AW41" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AX41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AY41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="AZ41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="BA41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="BB41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="BC41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
     </row>
@@ -5082,220 +5301,220 @@
       <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B42" s="19" t="str">
+      <c r="B42" s="16" t="str">
         <f>IF(B21="1.6",IF($B11 ="Sechskant",B41+B35,IF($B11="Zylinderkopf",B31+B41,IF($B11="Senkkopf",B40+B41,"0"))),"0")</f>
         <v>0</v>
       </c>
-      <c r="C42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(C21="2",IF($B11 ="Sechskant",C41+C35,IF($B11="Zylinderkopf",C31+C41,IF($B11="Senkkopf",C40+C41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="D42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(D21="2.5",IF($B11 ="Sechskant",D41+D35,IF($B11="Zylinderkopf",D31+D41,IF($B11="Senkkopf",D40+D41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="E42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(E21="3",IF($B11 ="Sechskant",E41+E35,IF($B11="Zylinderkopf",E31+E41,IF($B11="Senkkopf",E40+E41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="F42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(F21="4",IF($B11 ="Sechskant",F41+F35,IF($B11="Zylinderkopf",F31+F41,IF($B11="Senkkopf",F40+F41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="G42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(G21="5",IF($B11 ="Sechskant",G41+G35,IF($B11="Zylinderkopf",G31+G41,IF($B11="Senkkopf",G40+G41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="H42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(H21="6",IF($B11 ="Sechskant",H41+H35,IF($B11="Zylinderkopf",H31+H41,IF($B11="Senkkopf",H40+H41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="I42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(I21="8",IF($B11 ="Sechskant",I41+I35,IF($B11="Zylinderkopf",I31+I41,IF($B11="Senkkopf",I40+I41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(J21="10",IF($B11 ="Sechskant",J41+J35,IF($B11="Zylinderkopf",J31+J41,IF($B11="Senkkopf",J40+J41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(K21="12",IF($B11 ="Sechskant",K41+K35,IF($B11="Zylinderkopf",K31+K41,IF($B11="Senkkopf",K40+K41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="L42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(L21="16",IF($B11 ="Sechskant",L41+L35,IF($B11="Zylinderkopf",L31+L41,IF($B11="Senkkopf",L40+L41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(M21="20",IF($B11 ="Sechskant",M41+M35,IF($B11="Zylinderkopf",M31+M41,IF($B11="Senkkopf",M40+M41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(N21="24",IF($B11 ="Sechskant",N41+N35,IF($B11="Zylinderkopf",N31+N41,IF($B11="Senkkopf",N40+N41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(O21="30",IF($B11 ="Sechskant",O41+O35,IF($B11="Zylinderkopf",O31+O41,IF($B11="Senkkopf",O40+O41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="P42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(P21="36",IF($B11 ="Sechskant",P41+P35,IF($B11="Zylinderkopf",P31+P41,IF($B11="Senkkopf",P40+P41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q42" s="1">
-        <f>IF($B9&gt;0,IF(Q21="42",IF($B11 ="Sechskant",Q41+Q35,IF($B11="Zylinderkopf",Q31+Q41,IF($B11="Senkkopf",Q40+Q41,"0")))),0)</f>
-        <v>1480575.2508388194</v>
-      </c>
-      <c r="R42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(R21="2",IF($B11 ="Sechskant",R41+R35,IF($B11="Zylinderkopf",R31+R41,IF($B11="Senkkopf",R40+R41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="S42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(S21="3",IF($B11 ="Sechskant",S41+S35,IF($B11="Zylinderkopf",S31+S41,IF($B11="Senkkopf",S40+S41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="T42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(T21="4",IF($B11 ="Sechskant",T41+T35,IF($B11="Zylinderkopf",T31+T41,IF($B11="Senkkopf",T40+T41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="U42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(U21="4",IF($B11 ="Sechskant",U41+U35,IF($B11="Zylinderkopf",U31+U41,IF($B11="Senkkopf",U40+U41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="V42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(V21="5",IF($B11 ="Sechskant",V41+V35,IF($B11="Zylinderkopf",V31+V41,IF($B11="Senkkopf",V40+V41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="W42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(W21="5",IF($B11 ="Sechskant",W41+W35,IF($B11="Zylinderkopf",W31+W41,IF($B11="Senkkopf",W40+W41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="X42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(X21="6",IF($B11 ="Sechskant",X41+X35,IF($B11="Zylinderkopf",X31+X41,IF($B11="Senkkopf",X40+X41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y42" s="1" t="b">
-        <f t="shared" ref="Y42:Z42" si="16">IF($B9&gt;0,IF(Y21="6",IF($B11 ="Sechskant",Y41+Y35,IF($B11="Zylinderkopf",Y31+Y41,IF($B11="Senkkopf",Y40+Y41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z42" s="1" t="b">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="AA42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AA21="8",IF($B11 ="Sechskant",AA41+AA35,IF($B11="Zylinderkopf",AA31+AA41,IF($B11="Senkkopf",AA40+AA41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AB42" s="1" t="b">
-        <f t="shared" ref="AB42:AC42" si="17">IF($B9&gt;0,IF(AB21="8",IF($B11 ="Sechskant",AB41+AB35,IF($B11="Zylinderkopf",AB31+AB41,IF($B11="Senkkopf",AB40+AB41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC42" s="1" t="b">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="AD42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AD21="10",IF($B11 ="Sechskant",AD41+AD35,IF($B11="Zylinderkopf",AD31+AD41,IF($B11="Senkkopf",AD40+AD41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AE42" s="1" t="b">
-        <f t="shared" ref="AE42:AF42" si="18">IF($B9&gt;0,IF(AE21="10",IF($B11 ="Sechskant",AE41+AE35,IF($B11="Zylinderkopf",AE31+AE41,IF($B11="Senkkopf",AE40+AE41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AF42" s="1" t="b">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AG42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AG21="12",IF($B11 ="Sechskant",AG41+AG35,IF($B11="Zylinderkopf",AG31+AG41,IF($B11="Senkkopf",AG40+AG41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AH42" s="1" t="b">
-        <f t="shared" ref="AH42:AI42" si="19">IF($B9&gt;0,IF(AH21="12",IF($B11 ="Sechskant",AH41+AH35,IF($B11="Zylinderkopf",AH31+AH41,IF($B11="Senkkopf",AH40+AH41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AI42" s="1" t="b">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="AJ42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AJ21="16",IF($B11 ="Sechskant",AJ41+AJ35,IF($B11="Zylinderkopf",AJ31+AJ41,IF($B11="Senkkopf",AJ40+AJ41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AK42" s="1" t="b">
-        <f t="shared" ref="AK42:AL42" si="20">IF($B9&gt;0,IF(AK21="16",IF($B11 ="Sechskant",AK41+AK35,IF($B11="Zylinderkopf",AK31+AK41,IF($B11="Senkkopf",AK40+AK41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AL42" s="1" t="b">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AM42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AM21="20",IF($B11 ="Sechskant",AM41+AM35,IF($B11="Zylinderkopf",AM31+AM41,IF($B11="Senkkopf",AM40+AM41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AN42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AN21="20",IF($B11 ="Sechskant",AN41+AN35,IF($B11="Zylinderkopf",AN31+AN41,IF($B11="Senkkopf",AN40+AN41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AO42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AO21="24",IF($B11 ="Sechskant",AO41+AO35,IF($B11="Zylinderkopf",AO31+AO41,IF($B11="Senkkopf",AO40+AO41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AP42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AP21="24",IF($B11 ="Sechskant",AP41+AP35,IF($B11="Zylinderkopf",AP31+AP41,IF($B11="Senkkopf",AP40+AP41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AQ42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AQ21="30",IF($B11 ="Sechskant",AQ41+AQ35,IF($B11="Zylinderkopf",AQ31+AQ41,IF($B11="Senkkopf",AQ40+AQ41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AR42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AR21="30",IF($B11 ="Sechskant",AR41+AR35,IF($B11="Zylinderkopf",AR31+AR41,IF($B11="Senkkopf",AR40+AR41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AS42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AS21="36",IF($B11 ="Sechskant",AS41+AS35,IF($B11="Zylinderkopf",AS31+AS41,IF($B11="Senkkopf",AS40+AS41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AT42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AT21="36",IF($B11 ="Sechskant",AT41+AT35,IF($B11="Zylinderkopf",AT31+AT41,IF($B11="Senkkopf",AT40+AT41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AU42" s="1" t="b">
-        <f t="shared" ref="AU42:AV42" si="21">IF($B9&gt;0,IF(AU21="42",IF($B11 ="Sechskant",AU41+AU35,IF($B11="Zylinderkopf",AU31+AU41,IF($B11="Senkkopf",AU40+AU41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AV42" s="1" t="b">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="AW42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AW21="6.35",IF($B11 ="Sechskant",AW41+AW35,IF($B11="Zylinderkopf",AW31+AW41,IF($B11="Senkkopf",AW40+AW41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AX42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AX21="9.53",IF($B11 ="Sechskant",AX41+AX35,IF($B11="Zylinderkopf",AX31+AX41,IF($B11="Senkkopf",AX40+AX41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AY42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AY21="12.7",IF($B11 ="Sechskant",AY41+AY35,IF($B11="Zylinderkopf",AY31+AY41,IF($B11="Senkkopf",AY40+AY41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AZ42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(AZ21="19.05",IF($B11 ="Sechskant",AZ41+AZ35,IF($B11="Zylinderkopf",AZ31+AZ41,IF($B11="Senkkopf",AZ40+AZ41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BA42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(BA21="25.4",IF($B11 ="Sechskant",BA41+BA35,IF($B11="Zylinderkopf",BA31+BA41,IF($B11="Senkkopf",BA40+BA41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BB42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(BB21="31.75",IF($B11 ="Sechskant",BB41+BB35,IF($B11="Zylinderkopf",BB31+BB41,IF($B11="Senkkopf",BB40+BB41,"0")))),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BC42" s="1" t="b">
-        <f>IF($B9&gt;0,IF(BC21="38.1",IF($B11 ="Sechskant",BC41+BC35,IF($B11="Zylinderkopf",BC31+BC41,IF($B11="Senkkopf",BC40+BC41,"0")))),0)</f>
+      <c r="C42" s="1">
+        <f>IF($B9&gt;0,IF(C21="2",IF($B11 ="Sechskant",C41+C35,IF($B11="Zylinderkopf",C31+C41,IF($B11="Senkkopf",C40+C41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D42" s="1">
+        <f>IF($B9&gt;0,IF(D21="2.5",IF($B11 ="Sechskant",D41+D35,IF($B11="Zylinderkopf",D31+D41,IF($B11="Senkkopf",D40+D41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E42" s="1">
+        <f>IF($B9&gt;0,IF(E21="3",IF($B11 ="Sechskant",E41+E35,IF($B11="Zylinderkopf",E31+E41,IF($B11="Senkkopf",E40+E41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <f>IF($B9&gt;0,IF(F21="4",IF($B11 ="Sechskant",F41+F35,IF($B11="Zylinderkopf",F31+F41,IF($B11="Senkkopf",F40+F41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
+        <f>IF($B9&gt;0,IF(G21="5",IF($B11 ="Sechskant",G41+G35,IF($B11="Zylinderkopf",G31+G41,IF($B11="Senkkopf",G40+G41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <f>IF($B9&gt;0,IF(H21="6",IF($B11 ="Sechskant",H41+H35,IF($B11="Zylinderkopf",H31+H41,IF($B11="Senkkopf",H40+H41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I42" s="1">
+        <f>IF($B9&gt;0,IF(I21="8",IF($B11 ="Sechskant",I41+I35,IF($B11="Zylinderkopf",I31+I41,IF($B11="Senkkopf",I40+I41,"0"))),0),0)</f>
+        <v>51041.181411606405</v>
+      </c>
+      <c r="J42" s="1">
+        <f>IF($B9&gt;0,IF(J21="10",IF($B11 ="Sechskant",J41+J35,IF($B11="Zylinderkopf",J31+J41,IF($B11="Senkkopf",J40+J41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K42" s="1">
+        <f>IF($B9&gt;0,IF(K21="12",IF($B11 ="Sechskant",K41+K35,IF($B11="Zylinderkopf",K31+K41,IF($B11="Senkkopf",K40+K41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L42" s="1">
+        <f>IF($B9&gt;0,IF(L21="16",IF($B11 ="Sechskant",L41+L35,IF($B11="Zylinderkopf",L31+L41,IF($B11="Senkkopf",L40+L41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M42" s="1">
+        <f>IF($B9&gt;0,IF(M21="20",IF($B11 ="Sechskant",M41+M35,IF($B11="Zylinderkopf",M31+M41,IF($B11="Senkkopf",M40+M41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N42" s="1">
+        <f>IF($B9&gt;0,IF(N21="24",IF($B11 ="Sechskant",N41+N35,IF($B11="Zylinderkopf",N31+N41,IF($B11="Senkkopf",N40+N41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O42" s="1">
+        <f>IF($B9&gt;0,IF(O21="30",IF($B11 ="Sechskant",O41+O35,IF($B11="Zylinderkopf",O31+O41,IF($B11="Senkkopf",O40+O41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P42" s="1">
+        <f>IF($B9&gt;0,IF(P21="36",IF($B11 ="Sechskant",P41+P35,IF($B11="Zylinderkopf",P31+P41,IF($B11="Senkkopf",P40+P41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q42" s="13">
+        <f>IF($B9&gt;0,IF(Q21="42",IF($B11 ="Sechskant",Q41+Q35,IF($B11="Zylinderkopf",Q31+Q41,IF($B11="Senkkopf",Q40+Q41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R42" s="15">
+        <f>IF($B9&gt;0,IF(R21="2",IF($B11 ="Sechskant",R41+R35,IF($B11="Zylinderkopf",R31+R41,IF($B11="Senkkopf",R40+R41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S42" s="1">
+        <f>IF($B9&gt;0,IF(S21="3",IF($B11 ="Sechskant",S41+S35,IF($B11="Zylinderkopf",S31+S41,IF($B11="Senkkopf",S40+S41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T42" s="1">
+        <f>IF($B9&gt;0,IF(T21="4",IF($B11 ="Sechskant",T41+T35,IF($B11="Zylinderkopf",T31+T41,IF($B11="Senkkopf",T40+T41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U42" s="1">
+        <f>IF($B9&gt;0,IF(U21="4",IF($B11 ="Sechskant",U41+U35,IF($B11="Zylinderkopf",U31+U41,IF($B11="Senkkopf",U40+U41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V42" s="1">
+        <f>IF($B9&gt;0,IF(V21="5",IF($B11 ="Sechskant",V41+V35,IF($B11="Zylinderkopf",V31+V41,IF($B11="Senkkopf",V40+V41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W42" s="1">
+        <f>IF($B9&gt;0,IF(W21="5",IF($B11 ="Sechskant",W41+W35,IF($B11="Zylinderkopf",W31+W41,IF($B11="Senkkopf",W40+W41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X42" s="1">
+        <f>IF($B9&gt;0,IF(X21="6",IF($B11 ="Sechskant",X41+X35,IF($B11="Zylinderkopf",X31+X41,IF($B11="Senkkopf",X40+X41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y42" s="1">
+        <f>IF($B9&gt;0,IF(Y21="6",IF($B11 ="Sechskant",Y41+Y35,IF($B11="Zylinderkopf",Y31+Y41,IF($B11="Senkkopf",Y40+Y41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z42" s="1">
+        <f>IF($B9&gt;0,IF(Z21="6",IF($B11 ="Sechskant",Z41+Z35,IF($B11="Zylinderkopf",Z31+Z41,IF($B11="Senkkopf",Z40+Z41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA42" s="1">
+        <f>IF($B9&gt;0,IF(AA21="8",IF($B11 ="Sechskant",AA41+AA35,IF($B11="Zylinderkopf",AA31+AA41,IF($B11="Senkkopf",AA40+AA41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB42" s="1">
+        <f>IF($B9&gt;0,IF(AB21="8",IF($B11 ="Sechskant",AB41+AB35,IF($B11="Zylinderkopf",AB31+AB41,IF($B11="Senkkopf",AB40+AB41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC42" s="1">
+        <f>IF($B9&gt;0,IF(AC21="8",IF($B11 ="Sechskant",AC41+AC35,IF($B11="Zylinderkopf",AC31+AC41,IF($B11="Senkkopf",AC40+AC41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD42" s="1">
+        <f>IF($B9&gt;0,IF(AD21="10",IF($B11 ="Sechskant",AD41+AD35,IF($B11="Zylinderkopf",AD31+AD41,IF($B11="Senkkopf",AD40+AD41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE42" s="1">
+        <f>IF($B9&gt;0,IF(AE21="10",IF($B11 ="Sechskant",AE41+AE35,IF($B11="Zylinderkopf",AE31+AE41,IF($B11="Senkkopf",AE40+AE41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF42" s="1">
+        <f>IF($B9&gt;0,IF(AF21="10",IF($B11 ="Sechskant",AF41+AF35,IF($B11="Zylinderkopf",AF31+AF41,IF($B11="Senkkopf",AF40+AF41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AG42" s="1">
+        <f>IF($B9&gt;0,IF(AG21="12",IF($B11 ="Sechskant",AG41+AG35,IF($B11="Zylinderkopf",AG31+AG41,IF($B11="Senkkopf",AG40+AG41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH42" s="1">
+        <f>IF($B9&gt;0,IF(AH21="12",IF($B11 ="Sechskant",AH41+AH35,IF($B11="Zylinderkopf",AH31+AH41,IF($B11="Senkkopf",AH40+AH41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI42" s="1">
+        <f>IF($B9&gt;0,IF(AI21="12",IF($B11 ="Sechskant",AI41+AI35,IF($B11="Zylinderkopf",AI31+AI41,IF($B11="Senkkopf",AI40+AI41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ42" s="1">
+        <f>IF($B9&gt;0,IF(AJ21="16",IF($B11 ="Sechskant",AJ41+AJ35,IF($B11="Zylinderkopf",AJ31+AJ41,IF($B11="Senkkopf",AJ40+AJ41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AK42" s="1">
+        <f>IF($B9&gt;0,IF(AK21="16",IF($B11 ="Sechskant",AK41+AK35,IF($B11="Zylinderkopf",AK31+AK41,IF($B11="Senkkopf",AK40+AK41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AL42" s="1">
+        <f>IF($B9&gt;0,IF(AL21="16",IF($B11 ="Sechskant",AL41+AL35,IF($B11="Zylinderkopf",AL31+AL41,IF($B11="Senkkopf",AL40+AL41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AM42" s="1">
+        <f>IF($B9&gt;0,IF(AM21="20",IF($B11 ="Sechskant",AM41+AM35,IF($B11="Zylinderkopf",AM31+AM41,IF($B11="Senkkopf",AM40+AM41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN42" s="1">
+        <f>IF($B9&gt;0,IF(AN21="20",IF($B11 ="Sechskant",AN41+AN35,IF($B11="Zylinderkopf",AN31+AN41,IF($B11="Senkkopf",AN40+AN41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO42" s="1">
+        <f>IF($B9&gt;0,IF(AO21="24",IF($B11 ="Sechskant",AO41+AO35,IF($B11="Zylinderkopf",AO31+AO41,IF($B11="Senkkopf",AO40+AO41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AP42" s="1">
+        <f>IF($B9&gt;0,IF(AP21="24",IF($B11 ="Sechskant",AP41+AP35,IF($B11="Zylinderkopf",AP31+AP41,IF($B11="Senkkopf",AP40+AP41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ42" s="1">
+        <f>IF($B9&gt;0,IF(AQ21="30",IF($B11 ="Sechskant",AQ41+AQ35,IF($B11="Zylinderkopf",AQ31+AQ41,IF($B11="Senkkopf",AQ40+AQ41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AR42" s="1">
+        <f>IF($B9&gt;0,IF(AR21="30",IF($B11 ="Sechskant",AR41+AR35,IF($B11="Zylinderkopf",AR31+AR41,IF($B11="Senkkopf",AR40+AR41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AS42" s="1">
+        <f>IF($B9&gt;0,IF(AS21="36",IF($B11 ="Sechskant",AS41+AS35,IF($B11="Zylinderkopf",AS31+AS41,IF($B11="Senkkopf",AS40+AS41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AT42" s="1">
+        <f>IF($B9&gt;0,IF(AT21="36",IF($B11 ="Sechskant",AT41+AT35,IF($B11="Zylinderkopf",AT31+AT41,IF($B11="Senkkopf",AT40+AT41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AU42" s="1">
+        <f>IF($B9&gt;0,IF(AU21="42",IF($B11 ="Sechskant",AU41+AU35,IF($B11="Zylinderkopf",AU31+AU41,IF($B11="Senkkopf",AU40+AU41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AV42" s="5">
+        <f>IF($B9&gt;0,IF(AV21="42",IF($B11 ="Sechskant",AV41+AV35,IF($B11="Zylinderkopf",AV31+AV41,IF($B11="Senkkopf",AV40+AV41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AW42" s="6">
+        <f>IF($B9&gt;0,IF(AW21="6.35",IF($B11 ="Sechskant",AW41+AW35,IF($B11="Zylinderkopf",AW31+AW41,IF($B11="Senkkopf",AW40+AW41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AX42" s="1">
+        <f>IF($B9&gt;0,IF(AX21="9.53",IF($B11 ="Sechskant",AX41+AX35,IF($B11="Zylinderkopf",AX31+AX41,IF($B11="Senkkopf",AX40+AX41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AY42" s="1">
+        <f>IF($B9&gt;0,IF(AY21="12.7",IF($B11 ="Sechskant",AY41+AY35,IF($B11="Zylinderkopf",AY31+AY41,IF($B11="Senkkopf",AY40+AY41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ42" s="1">
+        <f>IF($B9&gt;0,IF(AZ21="19.05",IF($B11 ="Sechskant",AZ41+AZ35,IF($B11="Zylinderkopf",AZ31+AZ41,IF($B11="Senkkopf",AZ40+AZ41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BA42" s="1">
+        <f>IF($B9&gt;0,IF(BA21="25.4",IF($B11 ="Sechskant",BA41+BA35,IF($B11="Zylinderkopf",BA31+BA41,IF($B11="Senkkopf",BA40+BA41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BB42" s="1">
+        <f>IF($B9&gt;0,IF(BB21="31.75",IF($B11 ="Sechskant",BB41+BB35,IF($B11="Zylinderkopf",BB31+BB41,IF($B11="Senkkopf",BB40+BB41,"0"))),0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="BC42" s="1">
+        <f>IF($B9&gt;0,IF(BC21="38.1",IF($B11 ="Sechskant",BC41+BC35,IF($B11="Zylinderkopf",BC31+BC41,IF($B11="Senkkopf",BC40+BC41,"0"))),0),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5303,220 +5522,220 @@
       <c r="A43" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="19">
-        <f t="shared" ref="B43:BC43" si="22">IF($B8="Stahl",$B3,IF($B8="Aluminium",$C3,IF($B8="Titan",$D3,IF($B8="Messing",$E3,IF($B8="Kupfer",$F3,IF($B8="Bronze",$G3,"0"))))))*B42</f>
+      <c r="B43" s="16">
+        <f t="shared" ref="B43:BC43" si="64">IF($B8="Stahl",$B3,IF($B8="Aluminium",$C3,IF($B8="Titan",$D3,IF($B8="Messing",$E3,IF($B8="Kupfer",$F3,IF($B8="Bronze",$G3,"0"))))))*B42</f>
         <v>0</v>
       </c>
       <c r="C43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="E43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="F43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="G43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="H43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I43" s="1">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <f t="shared" si="64"/>
+        <v>400.67327408111026</v>
       </c>
       <c r="J43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="K43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="L43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="M43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="N43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="O43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="P43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="Q43" s="13">
-        <f t="shared" si="22"/>
-        <v>11622.515719084731</v>
+        <f t="shared" si="64"/>
+        <v>0</v>
       </c>
       <c r="R43" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="S43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="T43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="U43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="V43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="W43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="X43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="Y43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="Z43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AA43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AB43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AC43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AD43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AE43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AF43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AG43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AH43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AI43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AJ43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AK43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AL43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AM43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AN43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AO43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AP43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AQ43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AR43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AS43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AT43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AU43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AV43" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AW43" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AX43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AY43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="AZ43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="BA43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="BB43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="BC43" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
     </row>
@@ -5524,220 +5743,220 @@
       <c r="A44" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="19">
-        <f t="shared" ref="B44:BC44" si="23">($B14*B43)/1000</f>
+      <c r="B44" s="16">
+        <f t="shared" ref="B44:BC44" si="65">($B14*B43)/1000</f>
         <v>0</v>
       </c>
       <c r="C44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="E44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="F44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="G44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="H44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="I44" s="1">
-        <f t="shared" si="23"/>
-        <v>0</v>
+        <f t="shared" si="65"/>
+        <v>20.033663704055513</v>
       </c>
       <c r="J44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="K44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="L44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="M44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="N44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="O44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="P44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="Q44" s="13">
-        <f t="shared" si="23"/>
-        <v>581.12578595423656</v>
+        <f t="shared" si="65"/>
+        <v>0</v>
       </c>
       <c r="R44" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="S44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="T44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="U44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="V44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="W44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="X44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="Y44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="Z44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AA44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AB44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AC44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AD44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AE44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AF44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AG44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AH44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AI44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AJ44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AK44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AL44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AM44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AN44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AO44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AP44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AQ44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AR44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AS44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AT44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AU44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AV44" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AW44" s="6">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AX44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AY44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="AZ44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="BA44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="BB44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="BC44" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
     </row>
@@ -5751,12 +5970,12 @@
         <v>47</v>
       </c>
       <c r="B50" s="10">
-        <f>B21+C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21+Q21+R21+S21+T21+U21+V21+W21+X21+Y21+Z21+AA21+AB21+AC21+AD21+AE21+AF21+AG21+AI21+AH21+AJ21+AK21+AL21+AM21+AN21+AO21+AP21+AQ21+AR21+AS21+AT21+AU21+AV21+AW21+AX21+AY21+AZ21+BA21+BB21+BC21</f>
-        <v>42</v>
-      </c>
-      <c r="C50" s="24">
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21+Q21+R21+S21+T21+U21+V21+W21+X21+Y21+Z21+AA21+AB21+AC21+AD21+AE21+AF21+AG21+AI21+AH21+AJ21+AK21+AL21+AM21+AN21+AO21+AP21+AQ21+AR21+AS21+AT21+AU21+AV21+AW21+AX21+AY21+AZ21+BA21+BB21+BC21</f>
+        <v>8</v>
+      </c>
+      <c r="C50" s="21">
         <f>B50</f>
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D50" s="12"/>
     </row>
@@ -5765,12 +5984,12 @@
         <v>48</v>
       </c>
       <c r="B51" s="10">
-        <f>B22+C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22+Q22+R22+S22+T22+U22+V22+W22+X22+Y22+Z22+AA22+AB22+AC22+AD22+AE22+AF22+AG22+AH22+AI22+AJ22+AK22+AL22+AM22+AN22+AO22+AP22+AQ22+AR22+AS22+AT22+AU22+AV22+AW22+AX22+AY22+AZ22+BA22+BB22+BC22</f>
-        <v>4.5</v>
-      </c>
-      <c r="C51" s="24">
-        <f t="shared" ref="C51:C54" si="24">B51</f>
-        <v>4.5</v>
+        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22+Q22+R22+S22+T22+U22+V22+W22+X22+Y22+Z22+AA22+AB22+AC22+AD22+AE22+AF22+AG22+AH22+AI22+AJ22+AK22+AL22+AM22+AN22+AO22+AP22+AQ22+AR22+AS22+AT22+AU22+AV22+AW22+AX22+AY22+AZ22+BA22+BB22+BC22</f>
+        <v>1.25</v>
+      </c>
+      <c r="C51" s="21">
+        <f t="shared" ref="C51:C54" si="66">B51</f>
+        <v>1.25</v>
       </c>
       <c r="D51" s="12"/>
     </row>
@@ -5779,12 +5998,12 @@
         <v>49</v>
       </c>
       <c r="B52" s="10">
-        <f>MAX(B23:AV23)+AW23+AX23+AY23+AZ23+BA23+BB23+BC23</f>
-        <v>39.077249999999999</v>
-      </c>
-      <c r="C52" s="24">
-        <f t="shared" si="24"/>
-        <v>39.077249999999999</v>
+        <f>MAX(C23:AV23)+AW23+AX23+AY23+AZ23+BA23+BB23+BC23</f>
+        <v>7.1881250000000003</v>
+      </c>
+      <c r="C52" s="21">
+        <f t="shared" si="66"/>
+        <v>7.1881250000000003</v>
       </c>
       <c r="D52" s="12"/>
     </row>
@@ -5793,12 +6012,12 @@
         <v>50</v>
       </c>
       <c r="B53" s="10">
-        <f>MAX(B24:AV24)+AW24+AX24+AY24+AZ24+BA24+BB24+BC24</f>
-        <v>36.478949999999998</v>
-      </c>
-      <c r="C53" s="24">
-        <f t="shared" si="24"/>
-        <v>36.478949999999998</v>
+        <f>MAX(C24:AV24)+AW24+AX24+AY24+AZ24+BA24+BB24+BC24</f>
+        <v>6.4663749999999993</v>
+      </c>
+      <c r="C53" s="21">
+        <f t="shared" si="66"/>
+        <v>6.4663749999999993</v>
       </c>
       <c r="D53" s="12"/>
     </row>
@@ -5807,12 +6026,12 @@
         <v>51</v>
       </c>
       <c r="B54" s="10">
-        <f>MAX(B25:AV25)+AW25+AX25+AY25+AZ25+BA25+BB25+BC25</f>
-        <v>37.5</v>
-      </c>
-      <c r="C54" s="24">
-        <f t="shared" si="24"/>
-        <v>37.5</v>
+        <f>MAX(C25:AV25)+AW25+AX25+AY25+AZ25+BA25+BB25+BC25</f>
+        <v>6.75</v>
+      </c>
+      <c r="C54" s="21">
+        <f t="shared" si="66"/>
+        <v>6.75</v>
       </c>
       <c r="D54" s="12"/>
     </row>
@@ -5821,12 +6040,12 @@
         <v>69</v>
       </c>
       <c r="B55" s="10">
-        <f>B44+C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44+Q44+R44+S44+T44+U44+V44+W44+X44+Y44+Z44+AA44+AB44+AC44+AD44+AE44+AF44+AG44+AH44+AI44+AJ44+AK44+AL44+AM44+AN44+AO44+AP44+AQ44+AR44+AS44+AT44+AU44+AV44+AW44+AX44+AY44+AZ44+BA44+BB44+BC44</f>
-        <v>581.12578595423656</v>
-      </c>
-      <c r="C55" s="25">
+        <f>C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44+Q44+R44+S44+T44+U44+V44+W44+X44+Y44+Z44+AA44+AB44+AC44+AD44+AE44+AF44+AG44+AH44+AI44+AJ44+AK44+AL44+AM44+AN44+AO44+AP44+AQ44+AR44+AS44+AT44+AU44+AV44+AW44+AX44+AY44+AZ44+BA44+BB44+BC44</f>
+        <v>20.033663704055513</v>
+      </c>
+      <c r="C55" s="22">
         <f>B55</f>
-        <v>581.12578595423656</v>
+        <v>20.033663704055513</v>
       </c>
       <c r="D55" s="12"/>
     </row>
@@ -5835,18 +6054,18 @@
         <v>70</v>
       </c>
       <c r="B56" s="10">
-        <f>IF($B11 = "Sechskant",B34+C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34+Q34+R34+T34+S34+U34+V34+W34+X34+Y34+Z34+AA34+AB34+AC34+AD34+AE34+AF34+AG34+AH34+AI34+AJ34+AK34+AL34+AM34+AN34+AO34+AP34+AQ34+AR34+AS34+AT34+AU34+AV34+AW34+AX34+AY34+AZ34+BA34+BB34+BC34,IF($B11="Zylinderkopf",AW30+AX30+AY30+AZ30+BA30+B30+C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30+Q30+R30+S30+T30+U30+V30+W30+X30+Y30+AA30+Z30+AB30+AC30+AD30+AE30+AF30+AG30+AH30+AI30+AJ30+AK30+AL30+AM30+AN30+AO30+AP30+AQ30+AR30+AS30+AT30+AU30+AV30+BB30+BC30,IF(B11="Senkkopf",AW39+AX39+AY39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+S39+T39+U39+V39+W39+X39+Y39+Z39+AA39+AB39+AC39+AD39+AE39+AF39+AG39+AH39+AI39+AJ39+AK39+AL39+AM39+AN39+AO39+AP39,"0")))</f>
-        <v>65</v>
-      </c>
-      <c r="C56" s="30">
+        <f>IF($B11 = "Sechskant",C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34+Q34+R34+T34+S34+U34+V34+W34+X34+Y34+Z34+AA34+AB34+AC34+AD34+AE34+AF34+AG34+AH34+AI34+AJ34+AK34+AL34+AM34+AN34+AO34+AP34+AQ34+AR34+AS34+AT34+AU34+AV34+AW34+AX34+AY34+AZ34+BA34+BB34+BC34,IF($B11="Zylinderkopf",AW30+AX30+AY30+AZ30+BA30+C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30+Q30+R30+S30+T30+U30+V30+W30+X30+Y30+AA30+Z30+AB30+AC30+AD30+AE30+AF30+AG30+AH30+AI30+AJ30+AK30+AL30+AM30+AN30+AO30+AP30+AQ30+AR30+AS30+AT30+AU30+AV30+BB30+BC30,IF(B11="Senkkopf",AW39+AX39+AY39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+S39+T39+U39+V39+W39+X39+Y39+Z39+AA39+AB39+AC39+AD39+AE39+AF39+AG39+AH39+AI39+AJ39+AK39+AL39+AM39+AN39+AO39+AP39,"0")))</f>
+        <v>13</v>
+      </c>
+      <c r="C56" s="26">
         <f>D56</f>
-        <v>65</v>
-      </c>
-      <c r="D56" s="22">
+        <v>13</v>
+      </c>
+      <c r="D56" s="19">
         <f>IF(E56="0",B56,E56)</f>
-        <v>65</v>
-      </c>
-      <c r="E56" s="21" t="str">
+        <v>13</v>
+      </c>
+      <c r="E56" s="18" t="str">
         <f>IF(B56=3.97,"0.156",IF(B56=4.76,"0.188",IF(B56=5.56,"0.219",IF(B56=7.95,"5/16",IF(B56=9.52,"3/8",IF(B56=11.1,"7/16",IF(B56=14.3,"9/16",IF(B56=15.88,"5/8",IF(B56=19.05,"3/4",IF(B56=22.23,"7/8",IF(B56=25.4,"1",IF(B56=28.6,"1 1/8",IF(B56=38.1,"1 1/2",IF(B56=47.6,"1 7/8",IF(B56=57.2,"2  1/4","0")))))))))))))))</f>
         <v>0</v>
       </c>
@@ -5859,12 +6078,12 @@
         <f>IF(B50=0,"0",IF(B16="3.6","180",IF(B16="4.6","240",IF(B16="4.8","320",IF(B16="5.8","400",IF(B16="6.8","480",IF(B16="8.8","640",IF(B16="9.8","720",IF(B16="10.9","900",IF(B16="12.9","1080","0"))))))))))</f>
         <v>240</v>
       </c>
-      <c r="C57" s="29" t="str">
+      <c r="C57" s="25" t="str">
         <f>B57</f>
         <v>240</v>
       </c>
       <c r="D57" s="12"/>
-      <c r="F57" s="23"/>
+      <c r="F57" s="20"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -5874,7 +6093,7 @@
         <f>IF(B50=0,"0",IF(B16="3.6","300",IF(B16="4.6","400",IF(B16="4.8","400",IF(B16="5.8","500",IF(B16="6.8","600",IF(B16="8.8","800",IF(B16="9.8","900",IF(B16="10.9","1000",IF(B16="12.9","1200","0"))))))))))</f>
         <v>400</v>
       </c>
-      <c r="C58" s="29" t="str">
+      <c r="C58" s="25" t="str">
         <f>B58</f>
         <v>400</v>
       </c>
@@ -5886,15 +6105,15 @@
       </c>
       <c r="B59" s="10">
         <f>IF(B8="Stahl",B55*B4*4.25,IF(B8="Aluminium",B55*C4*4.25,IF(B8="Titan",B55*D4*4.25,IF(B8="Messing",B55*E4*4.25,IF(B8="Kupfer",B55*F4*4.25,IF(B8="Bronze",B55*G4*4.25,"0"))))))</f>
-        <v>1234.8922951527527</v>
-      </c>
-      <c r="C59" s="26">
+        <v>42.571535371117967</v>
+      </c>
+      <c r="C59" s="23">
         <f>D59</f>
-        <v>1234.8922951527527</v>
+        <v>47.571535371117967</v>
       </c>
       <c r="D59" s="12">
         <f>IF(B59&gt;=55,B59,B59+5)</f>
-        <v>1234.8922951527527</v>
+        <v>47.571535371117967</v>
       </c>
       <c r="F59" t="s">
         <v>74</v>
@@ -5914,38 +6133,72 @@
         <v>52</v>
       </c>
       <c r="B60" s="10">
-        <f>MAX(B26:BC26)</f>
-        <v>152745.02021569913</v>
-      </c>
-      <c r="C60" s="27">
+        <f>MAX(C26:BC26)</f>
+        <v>201.06192982974676</v>
+      </c>
+      <c r="C60" s="24">
         <f>B60</f>
-        <v>152745.02021569913</v>
+        <v>201.06192982974676</v>
       </c>
       <c r="D60" s="12"/>
     </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61">
+        <f>IF(B11 ="Zylinderkopf",C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28+Q28+R28+S28+T28+U28+V28+X28+W28+Y28+Z28+AA28+AB28+AC28+AD28+AE28+AF28+AG28+AH28+AI28+AJ28+AK28+AL28+AM28+AN28+AO28+AP28+AQ28+AR28+AS28+AT28+AU28+AV28+AW28+AX28+AY28+AZ28+BA28+BB28+BC28,IF(B11 = "Sechskant",C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33+Q33+R33+S33+T33+U33+V33+W33+X33+Y33+Z33+AA33+AB33+AC33+AD33+AE33+AF33+AG33+AH33+AI33+AJ33+AK33+AL33+AM33+AN33+AO33+AP33+AQ33+AR33+AS33+AT33+AU33+AV33+AW33+AX33+AY33+AZ33+BA33+BB33+BC33,IF(B11 ="Senkkopf",E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+S37+T37+U37+V37+W37+X37+Y37+Z37+AA37+AB37+AD37+AC37+AE37+AF37+AG37+AH37+AI37+AJ37+AK37+AL37+AM37+AN37+AO37+AP37+AW37+AX37+AY37,0)))</f>
+        <v>5.3</v>
+      </c>
+      <c r="C61" s="35">
+        <f>B61</f>
+        <v>5.3</v>
+      </c>
+    </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>54</v>
+      </c>
+      <c r="B62">
+        <f>IF(B11 ="Zylinderkopf",C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29+Q29+R29+S29+T29+U29+V29+W29+X29+Y29+Z29+AA29+AB29+AC29+AD29+AE29+AF29+AG29+AH29+AI29+AJ29+AK29+AL29+AM29+AN29+AO29+AP29+AQ29+AR29+AS29+AT29+AU29+AV29+AW29+AX29+AY29+AZ29+BA29+BB29+BC29,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C62" s="35">
+        <f>B62</f>
+        <v>0</v>
+      </c>
       <c r="J62" s="12"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B63" s="28"/>
+      <c r="A63" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="36">
+        <f>IF(B11 ="Senkkopf", E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+S38+T38+U38+V38+W38+X38+Y38+Z38+AA38+AB38+AC38+AD38+AE38+AF38+AG38+AH38+AI38+AJ38+AK38+AL38+AM38+AN38+AO38+AP38+AW38+AX38+AY38,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C63" s="35">
+        <f>B63</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="33" t="s">
+      <c r="C65" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="D65" s="33"/>
-      <c r="E65" s="33"/>
-      <c r="F65" s="33"/>
-      <c r="G65" s="33"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="29"/>
+      <c r="G65" s="29"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="33" t="s">
+      <c r="C66" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="D66" s="33"/>
-      <c r="E66" s="33"/>
-      <c r="F66" s="33"/>
-      <c r="G66" s="33"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
+      <c r="G66" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>